<commit_message>
update time series data till 12/31/2021
</commit_message>
<xml_diff>
--- a/data/time_series/annual_cashflows_data.xlsx
+++ b/data/time_series/annual_cashflows_data.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\UPS_MV\data\time_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E5445A-9B3D-4CD4-BB4A-37A6B709CCB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2C8723-B80B-4580-81DE-6784E4A9592A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F3CCDB8E-F5F3-42E2-A382-F3745238F716}"/>
+    <workbookView xWindow="29580" yWindow="1260" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{F3CCDB8E-F5F3-42E2-A382-F3745238F716}"/>
   </bookViews>
   <sheets>
     <sheet name="PBO" sheetId="1" r:id="rId1"/>
     <sheet name="Service Cost" sheetId="2" r:id="rId2"/>
     <sheet name="PVFB" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027456B0-4AAC-4E49-B406-E9435788ACC8}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,1362 +434,1363 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44561</v>
+        <v>44926</v>
       </c>
       <c r="B2">
         <v>0.5</v>
       </c>
       <c r="C2">
-        <v>1204791461.3399999</v>
+        <v>1213627245.4200001</v>
       </c>
       <c r="D2">
-        <v>262634078.86805475</v>
+        <v>262659142.11859041</v>
       </c>
       <c r="E2">
-        <v>423998690.65212816</v>
+        <v>424015774.05129546</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44926</v>
+        <v>45291</v>
       </c>
       <c r="B3">
         <v>1.5</v>
       </c>
       <c r="C3">
-        <v>1261684103.96</v>
+        <v>1269439337.4100001</v>
       </c>
       <c r="D3">
-        <v>293598811.95267481</v>
+        <v>293647149.88196254</v>
       </c>
       <c r="E3">
-        <v>457035869.00254059</v>
+        <v>457065275.86267245</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45291</v>
+        <v>45657</v>
       </c>
       <c r="B4">
         <v>2.5</v>
       </c>
       <c r="C4">
-        <v>1322496063.3699999</v>
+        <v>1329411806.5599999</v>
       </c>
       <c r="D4">
-        <v>325396054.59743112</v>
+        <v>325472217.7202239</v>
       </c>
       <c r="E4">
-        <v>488364113.72205102</v>
+        <v>488405515.40864128</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45657</v>
+        <v>46022</v>
       </c>
       <c r="B5">
         <v>3.5</v>
       </c>
       <c r="C5">
-        <v>1382472631.28</v>
+        <v>1388611025.73</v>
       </c>
       <c r="D5">
-        <v>357636538.34325933</v>
+        <v>357745042.83172649</v>
       </c>
       <c r="E5">
-        <v>516810890.43667734</v>
+        <v>516863212.12272674</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>46022</v>
+        <v>46387</v>
       </c>
       <c r="B6">
         <v>4.5</v>
       </c>
       <c r="C6">
-        <v>1441834863.8</v>
+        <v>1447252732.9300001</v>
       </c>
       <c r="D6">
-        <v>389867992.82166582</v>
+        <v>390014113.85726863</v>
       </c>
       <c r="E6">
-        <v>540895445.84166336</v>
+        <v>540963075.93295217</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>46387</v>
+        <v>46752</v>
       </c>
       <c r="B7">
         <v>5.5</v>
       </c>
       <c r="C7">
-        <v>1497751499.9100001</v>
+        <v>1502556821.4100001</v>
       </c>
       <c r="D7">
-        <v>421824066.83676833</v>
+        <v>422013825.0374046</v>
       </c>
       <c r="E7">
-        <v>563149236.18472266</v>
+        <v>563238770.2817446</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>46752</v>
+        <v>47118</v>
       </c>
       <c r="B8">
         <v>6.5</v>
       </c>
       <c r="C8">
-        <v>1547726201.1400001</v>
+        <v>1552050232.1099999</v>
       </c>
       <c r="D8">
-        <v>453083228.76911718</v>
+        <v>453322828.62352318</v>
       </c>
       <c r="E8">
-        <v>583233736.5429765</v>
+        <v>583346925.73878193</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>47118</v>
+        <v>47483</v>
       </c>
       <c r="B9">
         <v>7.5</v>
       </c>
       <c r="C9">
-        <v>1589102521.6800001</v>
+        <v>1593034537.02</v>
       </c>
       <c r="D9">
-        <v>483050223.38620663</v>
+        <v>483346116.48300433</v>
       </c>
       <c r="E9">
-        <v>600123509.97729051</v>
+        <v>600262968.05763745</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>47483</v>
+        <v>47848</v>
       </c>
       <c r="B10">
         <v>8.5</v>
       </c>
       <c r="C10">
-        <v>1624760223.71</v>
+        <v>1628726662.4400001</v>
       </c>
       <c r="D10">
-        <v>511747783.55574632</v>
+        <v>512106964.06418198</v>
       </c>
       <c r="E10">
-        <v>614261963.29772615</v>
+        <v>614431256.93380749</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>47848</v>
+        <v>48213</v>
       </c>
       <c r="B11">
         <v>9.5</v>
       </c>
       <c r="C11">
-        <v>1655599731.8900001</v>
+        <v>1660081684.1800001</v>
       </c>
       <c r="D11">
-        <v>539361412.8522445</v>
+        <v>539789358.94055665</v>
       </c>
       <c r="E11">
-        <v>626198496.54223931</v>
+        <v>626399997.06846392</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>48213</v>
+        <v>48579</v>
       </c>
       <c r="B12">
         <v>10.5</v>
       </c>
       <c r="C12">
-        <v>1680062491.04</v>
+        <v>1685320815.6700001</v>
       </c>
       <c r="D12">
-        <v>565225475.78990197</v>
+        <v>565726574.31639421</v>
       </c>
       <c r="E12">
-        <v>636984727.66776252</v>
+        <v>637224083.46310794</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>48579</v>
+        <v>48944</v>
       </c>
       <c r="B13">
         <v>11.5</v>
       </c>
       <c r="C13">
-        <v>1698265090.71</v>
+        <v>1703990977.27</v>
       </c>
       <c r="D13">
-        <v>588581223.07479978</v>
+        <v>589160498.98871207</v>
       </c>
       <c r="E13">
-        <v>646269169.76537323</v>
+        <v>646549908.19188178</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>48944</v>
+        <v>49309</v>
       </c>
       <c r="B14">
         <v>12.5</v>
       </c>
       <c r="C14">
-        <v>1709261484.5899999</v>
+        <v>1715411808.22</v>
       </c>
       <c r="D14">
-        <v>609029003.14335012</v>
+        <v>609690875.99307108</v>
       </c>
       <c r="E14">
-        <v>653679128.09410274</v>
+        <v>654004643.88014925</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>49309</v>
+        <v>49674</v>
       </c>
       <c r="B15">
         <v>13.5</v>
       </c>
       <c r="C15">
-        <v>1710585940.3699999</v>
+        <v>1717248496.4400001</v>
       </c>
       <c r="D15">
-        <v>627070862.27018416</v>
+        <v>627819121.28365505</v>
       </c>
       <c r="E15">
-        <v>658968169.17953229</v>
+        <v>659341735.95668685</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>49674</v>
+        <v>50040</v>
       </c>
       <c r="B16">
         <v>14.5</v>
       </c>
       <c r="C16">
-        <v>1707038833.55</v>
+        <v>1714174177.53</v>
       </c>
       <c r="D16">
-        <v>643001946.6930207</v>
+        <v>643839652.0939014</v>
       </c>
       <c r="E16">
-        <v>662868227.19537663</v>
+        <v>663292666.11693799</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>50040</v>
+        <v>50405</v>
       </c>
       <c r="B17">
         <v>15.5</v>
       </c>
       <c r="C17">
-        <v>1696227089</v>
+        <v>1703777499.29</v>
       </c>
       <c r="D17">
-        <v>656624504.63606274</v>
+        <v>657553816.45534825</v>
       </c>
       <c r="E17">
-        <v>667087655.27668583</v>
+        <v>667565374.02980375</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>50405</v>
+        <v>50770</v>
       </c>
       <c r="B18">
         <v>16.5</v>
       </c>
       <c r="C18">
-        <v>1679550885.01</v>
+        <v>1687725805.77</v>
       </c>
       <c r="D18">
-        <v>667830970.39621174</v>
+        <v>668853099.22501326</v>
       </c>
       <c r="E18">
-        <v>671666580.33637738</v>
+        <v>672200031.14548743</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>50770</v>
+        <v>51135</v>
       </c>
       <c r="B19">
         <v>17.5</v>
       </c>
       <c r="C19">
-        <v>1657636310.6199999</v>
+        <v>1666142611.4100001</v>
       </c>
       <c r="D19">
-        <v>677063908.48883176</v>
+        <v>678179158.23396182</v>
       </c>
       <c r="E19">
-        <v>675366947.85476351</v>
+        <v>675957099.92138398</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>51135</v>
+        <v>51501</v>
       </c>
       <c r="B20">
         <v>18.5</v>
       </c>
       <c r="C20">
-        <v>1631475390.97</v>
+        <v>1640558569.6800001</v>
       </c>
       <c r="D20">
-        <v>684505897.8794055</v>
+        <v>685713582.29591227</v>
       </c>
       <c r="E20">
-        <v>677533260.62664318</v>
+        <v>678178758.23305225</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>51501</v>
+        <v>51866</v>
       </c>
       <c r="B21">
         <v>19.5</v>
       </c>
       <c r="C21">
-        <v>1598958726.3499999</v>
+        <v>1608435694.3599999</v>
       </c>
       <c r="D21">
-        <v>690200183.10835409</v>
+        <v>691498472.09422243</v>
       </c>
       <c r="E21">
-        <v>677977389.5571543</v>
+        <v>678671493.26447356</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>51866</v>
+        <v>52231</v>
       </c>
       <c r="B22">
         <v>20.5</v>
       </c>
       <c r="C22">
-        <v>1563480484.0699999</v>
+        <v>1573397888.3099999</v>
       </c>
       <c r="D22">
-        <v>694373074.82569456</v>
+        <v>695759069.0108918</v>
       </c>
       <c r="E22">
-        <v>676598184.35184896</v>
+        <v>677334354.24249148</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>52231</v>
+        <v>52596</v>
       </c>
       <c r="B23">
         <v>21.5</v>
       </c>
       <c r="C23">
-        <v>1523850232.3399999</v>
+        <v>1534121579.9400001</v>
       </c>
       <c r="D23">
-        <v>696997876.98309791</v>
+        <v>698467634.44513285</v>
       </c>
       <c r="E23">
-        <v>673340112.69752216</v>
+        <v>674115982.06267798</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>52596</v>
+        <v>52962</v>
       </c>
       <c r="B24">
         <v>22.5</v>
       </c>
       <c r="C24">
-        <v>1482354519.6800001</v>
+        <v>1492897667.3299999</v>
       </c>
       <c r="D24">
-        <v>697824022.70833158</v>
+        <v>699372552.20554912</v>
       </c>
       <c r="E24">
-        <v>668389054.91703832</v>
+        <v>669200470.54096711</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>52962</v>
+        <v>53327</v>
       </c>
       <c r="B25">
         <v>23.5</v>
       </c>
       <c r="C25">
-        <v>1435259677.53</v>
+        <v>1446057869.3800001</v>
       </c>
       <c r="D25">
-        <v>696290143.69906712</v>
+        <v>697911404.50421655</v>
       </c>
       <c r="E25">
-        <v>661621285.5108633</v>
+        <v>662461057.13785613</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>53327</v>
+        <v>53692</v>
       </c>
       <c r="B26">
         <v>24.5</v>
       </c>
       <c r="C26">
-        <v>1383834164.77</v>
+        <v>1394912230.05</v>
       </c>
       <c r="D26">
-        <v>692263299.32491088</v>
+        <v>693950320.83901548</v>
       </c>
       <c r="E26">
-        <v>652890397.41032803</v>
+        <v>653748623.38036883</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>53692</v>
+        <v>54057</v>
       </c>
       <c r="B27">
         <v>25.5</v>
       </c>
       <c r="C27">
-        <v>1329867199.02</v>
+        <v>1341111105.48</v>
       </c>
       <c r="D27">
-        <v>686445051.58950925</v>
+        <v>688190164.6527648</v>
       </c>
       <c r="E27">
-        <v>642318916.72912443</v>
+        <v>643184810.84966457</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>54057</v>
+        <v>54423</v>
       </c>
       <c r="B28">
         <v>26.5</v>
       </c>
       <c r="C28">
-        <v>1271892300.79</v>
+        <v>1283077822.3499999</v>
       </c>
       <c r="D28">
-        <v>679015242.55001354</v>
+        <v>680810227.93361127</v>
       </c>
       <c r="E28">
-        <v>629850839.04606318</v>
+        <v>630714294.71687984</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>54423</v>
+        <v>54788</v>
       </c>
       <c r="B29">
         <v>27.5</v>
       </c>
       <c r="C29">
-        <v>1210269060.6800001</v>
+        <v>1221426484.76</v>
       </c>
       <c r="D29">
-        <v>669640962.33503735</v>
+        <v>671477097.23769784</v>
       </c>
       <c r="E29">
-        <v>615598525.00477409</v>
+        <v>616448234.49187398</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>54788</v>
+        <v>55153</v>
       </c>
       <c r="B30">
         <v>28.5</v>
       </c>
       <c r="C30">
-        <v>1145412617.8499999</v>
+        <v>1156480555.03</v>
       </c>
       <c r="D30">
-        <v>657921954.22511756</v>
+        <v>659790275.68906605</v>
       </c>
       <c r="E30">
-        <v>599751325.54945016</v>
+        <v>600573880.64061856</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>55153</v>
+        <v>55518</v>
       </c>
       <c r="B31">
         <v>29.5</v>
       </c>
       <c r="C31">
-        <v>1076404503.6700001</v>
+        <v>1087328191.0699999</v>
       </c>
       <c r="D31">
-        <v>643510723.73321092</v>
+        <v>645402297.92353272</v>
       </c>
       <c r="E31">
-        <v>588168131.71957743</v>
+        <v>588969020.39382529</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>55518</v>
+        <v>55884</v>
       </c>
       <c r="B32">
         <v>30.5</v>
       </c>
       <c r="C32">
-        <v>1008029899.3</v>
+        <v>1018731306.6</v>
       </c>
       <c r="D32">
-        <v>626939154.94546282</v>
+        <v>628845197.47830248</v>
       </c>
       <c r="E32">
-        <v>653387589.29023552</v>
+        <v>654617847.92331505</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>55884</v>
+        <v>56249</v>
       </c>
       <c r="B33">
         <v>31.5</v>
       </c>
       <c r="C33">
-        <v>935671684.97000003</v>
+        <v>946062645.11000001</v>
       </c>
       <c r="D33">
-        <v>608826593.11605942</v>
+        <v>610738672.94004881</v>
       </c>
       <c r="E33">
-        <v>698844972.77194655</v>
+        <v>700458249.75067556</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>56249</v>
+        <v>56614</v>
       </c>
       <c r="B34">
         <v>32.5</v>
       </c>
       <c r="C34">
-        <v>864422154.88999999</v>
+        <v>874426793.99000001</v>
       </c>
       <c r="D34">
-        <v>589558394.95561635</v>
+        <v>591468532.89777243</v>
       </c>
       <c r="E34">
-        <v>660420001.59486413</v>
+        <v>661931725.8571496</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>56614</v>
+        <v>56979</v>
       </c>
       <c r="B35">
         <v>33.5</v>
       </c>
       <c r="C35">
-        <v>795277596.66999996</v>
+        <v>804894914.36000001</v>
       </c>
       <c r="D35">
-        <v>569427676.29612637</v>
+        <v>571328378.64560461</v>
       </c>
       <c r="E35">
-        <v>621381776.77250683</v>
+        <v>622775801.94075274</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>56979</v>
+        <v>57345</v>
       </c>
       <c r="B36">
         <v>34.5</v>
       </c>
       <c r="C36">
-        <v>727284046.83000004</v>
+        <v>736476970.73000002</v>
       </c>
       <c r="D36">
-        <v>548691389.97646964</v>
+        <v>550575773.560853</v>
       </c>
       <c r="E36">
-        <v>582076475.15552306</v>
+        <v>583337433.7355845</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>57345</v>
+        <v>57710</v>
       </c>
       <c r="B37">
         <v>35.5</v>
       </c>
       <c r="C37">
-        <v>661931652.08000004</v>
+        <v>670670606.39999998</v>
       </c>
       <c r="D37">
-        <v>527499214.43699014</v>
+        <v>529361071.24776328</v>
       </c>
       <c r="E37">
-        <v>549820389.69532466</v>
+        <v>550942897.15521514</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>57710</v>
+        <v>58075</v>
       </c>
       <c r="B38">
         <v>36.5</v>
       </c>
       <c r="C38">
-        <v>600713631.44000006</v>
+        <v>608971991.13</v>
       </c>
       <c r="D38">
-        <v>506161620.12620246</v>
+        <v>507995421.29784733</v>
       </c>
       <c r="E38">
-        <v>519636701.80387092</v>
+        <v>520626161.2241593</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>58075</v>
+        <v>58440</v>
       </c>
       <c r="B39">
         <v>37.5</v>
       </c>
       <c r="C39">
-        <v>543503507.77999997</v>
+        <v>551270901.30999994</v>
       </c>
       <c r="D39">
-        <v>484849273.6292091</v>
+        <v>486650182.30266255</v>
       </c>
       <c r="E39">
-        <v>483785557.11718094</v>
+        <v>484646188.42140341</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>58440</v>
+        <v>58806</v>
       </c>
       <c r="B40">
         <v>38.5</v>
       </c>
       <c r="C40">
-        <v>489631585.82999998</v>
+        <v>496897872.72000003</v>
       </c>
       <c r="D40">
-        <v>463424680.29984099</v>
+        <v>465188469.71478313</v>
       </c>
       <c r="E40">
-        <v>448893140.57785767</v>
+        <v>449628286.54489565</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>58806</v>
+        <v>59171</v>
       </c>
       <c r="B41">
         <v>39.5</v>
       </c>
       <c r="C41">
-        <v>439631907.01999998</v>
+        <v>446392131.32999998</v>
       </c>
       <c r="D41">
-        <v>441310693.03812325</v>
+        <v>443033598.73878902</v>
       </c>
       <c r="E41">
-        <v>415173964.58602273</v>
+        <v>415783852.15479821</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>59171</v>
+        <v>59536</v>
       </c>
       <c r="B42">
         <v>40.5</v>
       </c>
       <c r="C42">
-        <v>393305841.63</v>
+        <v>399563847.73000002</v>
       </c>
       <c r="D42">
-        <v>418767068.6559965</v>
+        <v>420445956.41725731</v>
       </c>
       <c r="E42">
-        <v>382794997.85995734</v>
+        <v>383281984.03516048</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>59536</v>
+        <v>59901</v>
       </c>
       <c r="B43">
         <v>41.5</v>
       </c>
       <c r="C43">
-        <v>350515822.82999998</v>
+        <v>356279034.27999997</v>
       </c>
       <c r="D43">
-        <v>396762797.41653097</v>
+        <v>398395271.62121898</v>
       </c>
       <c r="E43">
-        <v>351880590.91962433</v>
+        <v>352252008.24275076</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>59901</v>
+        <v>60267</v>
       </c>
       <c r="B44">
         <v>42.5</v>
       </c>
       <c r="C44">
-        <v>311145280.41000003</v>
+        <v>316424106.57999998</v>
       </c>
       <c r="D44">
-        <v>375461785.23772132</v>
+        <v>377046021.55714232</v>
       </c>
       <c r="E44">
-        <v>322545517.51257885</v>
+        <v>322811822.83203197</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>60267</v>
+        <v>60632</v>
       </c>
       <c r="B45">
         <v>43.5</v>
       </c>
       <c r="C45">
-        <v>275091549.37</v>
+        <v>279903321.61000001</v>
       </c>
       <c r="D45">
-        <v>353466511.58123702</v>
+        <v>355000804.03109366</v>
       </c>
       <c r="E45">
-        <v>294865683.57015115</v>
+        <v>295036481.24885195</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>60632</v>
+        <v>60997</v>
       </c>
       <c r="B46">
         <v>44.5</v>
       </c>
       <c r="C46">
-        <v>242224263.16999999</v>
+        <v>246586556.37</v>
       </c>
       <c r="D46">
-        <v>330671756.08568138</v>
+        <v>332154553.53467178</v>
       </c>
       <c r="E46">
-        <v>268868833.65329564</v>
+        <v>268953117.07541275</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>60997</v>
+        <v>61362</v>
       </c>
       <c r="B47">
         <v>45.5</v>
       </c>
       <c r="C47">
-        <v>212391949.90000001</v>
+        <v>216326458.81999999</v>
       </c>
       <c r="D47">
-        <v>308492571.5501678</v>
+        <v>309922789.65834373</v>
       </c>
       <c r="E47">
-        <v>244548929.34735674</v>
+        <v>244555347.35137379</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>61362</v>
+        <v>61728</v>
       </c>
       <c r="B48">
         <v>46.5</v>
       </c>
       <c r="C48">
-        <v>185423082.74000001</v>
+        <v>188953210.80000001</v>
       </c>
       <c r="D48">
-        <v>287085695.3927772</v>
+        <v>288462425.10470229</v>
       </c>
       <c r="E48">
-        <v>221877002.58173776</v>
+        <v>221813807.83115515</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>61728</v>
+        <v>62093</v>
       </c>
       <c r="B49">
         <v>47.5</v>
       </c>
       <c r="C49">
-        <v>161127814.69999999</v>
+        <v>164278363.03999999</v>
       </c>
       <c r="D49">
-        <v>266466047.74623165</v>
+        <v>267788518.32217118</v>
       </c>
       <c r="E49">
-        <v>200809694.01692224</v>
+        <v>200684753.11110151</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>62093</v>
+        <v>62458</v>
       </c>
       <c r="B50">
         <v>48.5</v>
       </c>
       <c r="C50">
-        <v>139324600.22999999</v>
+        <v>142120875.03999999</v>
       </c>
       <c r="D50">
-        <v>246643354.27556399</v>
+        <v>247910874.3647587</v>
       </c>
       <c r="E50">
-        <v>181286179.74440762</v>
+        <v>181108394.59670976</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>62458</v>
+        <v>62823</v>
       </c>
       <c r="B51">
         <v>49.5</v>
       </c>
       <c r="C51">
-        <v>119832709.29000001</v>
+        <v>122300164.87</v>
       </c>
       <c r="D51">
-        <v>227627666.03523669</v>
+        <v>228839536.62758189</v>
       </c>
       <c r="E51">
-        <v>163240968.26349261</v>
+        <v>163019465.61501855</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>62823</v>
+        <v>63189</v>
       </c>
       <c r="B52">
         <v>50.5</v>
       </c>
       <c r="C52">
-        <v>102476825.41</v>
+        <v>104640857.15000001</v>
       </c>
       <c r="D52">
-        <v>209424932.47206366</v>
+        <v>210580402.0469687</v>
       </c>
       <c r="E52">
-        <v>146603067.26565558</v>
+        <v>146345463.57891101</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>63189</v>
+        <v>63554</v>
       </c>
       <c r="B53">
         <v>51.5</v>
       </c>
       <c r="C53">
-        <v>87089114.739999995</v>
+        <v>88974717.420000002</v>
       </c>
       <c r="D53">
-        <v>192038173.69757831</v>
+        <v>193136441.03002697</v>
       </c>
       <c r="E53">
-        <v>131293508.95752665</v>
+        <v>131006499.70167373</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>63554</v>
+        <v>63919</v>
       </c>
       <c r="B54">
         <v>52.5</v>
       </c>
       <c r="C54">
-        <v>73511609.549999997</v>
+        <v>75143356.760000005</v>
       </c>
       <c r="D54">
-        <v>175471233.67381138</v>
+        <v>176511591.38236633</v>
       </c>
       <c r="E54">
-        <v>117232487.54245569</v>
+        <v>116922505.81858487</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>63919</v>
+        <v>64284</v>
       </c>
       <c r="B55">
         <v>53.5</v>
       </c>
       <c r="C55">
-        <v>61595674.420000002</v>
+        <v>62997487.109999999</v>
       </c>
       <c r="D55">
-        <v>159728559.69934794</v>
+        <v>160710529.94410756</v>
       </c>
       <c r="E55">
-        <v>104343414.16807429</v>
+        <v>104016625.59105338</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>64284</v>
+        <v>64650</v>
       </c>
       <c r="B56">
         <v>54.5</v>
       </c>
       <c r="C56">
-        <v>51201347.090000004</v>
+        <v>52396035.57</v>
       </c>
       <c r="D56">
-        <v>144814596.11188632</v>
+        <v>145737855.10951975</v>
       </c>
       <c r="E56">
-        <v>92552755.582653418</v>
+        <v>92214859.748915792</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>64650</v>
+        <v>65015</v>
       </c>
       <c r="B57">
         <v>55.5</v>
       </c>
       <c r="C57">
-        <v>42196136.259999998</v>
+        <v>43205358.789999999</v>
       </c>
       <c r="D57">
-        <v>130733090.70836087</v>
+        <v>131597372.44534118</v>
       </c>
       <c r="E57">
-        <v>81790471.970618874</v>
+        <v>81446613.403591797</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>65015</v>
+        <v>65380</v>
       </c>
       <c r="B58">
         <v>56.5</v>
       </c>
       <c r="C58">
-        <v>34454303.310000002</v>
+        <v>35298638.060000002</v>
       </c>
       <c r="D58">
-        <v>117485915.94008407</v>
+        <v>118291129.90186666</v>
       </c>
       <c r="E58">
-        <v>71987633.500628784</v>
+        <v>71642420.750188708</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>65380</v>
+        <v>65745</v>
       </c>
       <c r="B59">
         <v>57.5</v>
       </c>
       <c r="C59">
-        <v>27855216.41</v>
+        <v>28554178.98</v>
       </c>
       <c r="D59">
-        <v>105072785.69463697</v>
+        <v>105819098.00988619</v>
       </c>
       <c r="E59">
-        <v>63086243.503159821</v>
+        <v>62743807.462651148</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>65745</v>
+        <v>66111</v>
       </c>
       <c r="B60">
         <v>58.5</v>
       </c>
       <c r="C60">
-        <v>22283689.640000001</v>
+        <v>22855775.390000001</v>
       </c>
       <c r="D60">
-        <v>93491570.528442055</v>
+        <v>94179444.085991025</v>
       </c>
       <c r="E60">
-        <v>55024822.767313123</v>
+        <v>54688813.412922546</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>66111</v>
+        <v>66476</v>
       </c>
       <c r="B61">
         <v>59.5</v>
       </c>
       <c r="C61">
-        <v>17629531.32</v>
+        <v>18092107.66</v>
       </c>
       <c r="D61">
-        <v>82737336.623664111</v>
+        <v>83367610.267755643</v>
       </c>
       <c r="E61">
-        <v>47747879.503264815</v>
+        <v>47421568.635305598</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>66476</v>
+        <v>66841</v>
       </c>
       <c r="B62">
         <v>60.5</v>
       </c>
       <c r="C62">
-        <v>13785284.68</v>
+        <v>14154394.720000001</v>
       </c>
       <c r="D62">
-        <v>72801169.216900662</v>
+        <v>73375064.046192244</v>
       </c>
       <c r="E62">
-        <v>41203428.489457466</v>
+        <v>40889651.017982721</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>66841</v>
+        <v>67206</v>
       </c>
       <c r="B63">
         <v>61.5</v>
       </c>
       <c r="C63">
-        <v>10648804.609999999</v>
+        <v>10939135.16</v>
       </c>
       <c r="D63">
-        <v>63669789.572720066</v>
+        <v>64188864.743345246</v>
       </c>
       <c r="E63">
-        <v>35342981.697424844</v>
+        <v>35044137.800875515</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>67206</v>
+        <v>67572</v>
       </c>
       <c r="B64">
         <v>62.5</v>
       </c>
       <c r="C64">
-        <v>8124576.7800000003</v>
+        <v>8349468.79</v>
       </c>
       <c r="D64">
-        <v>55325128.176718973</v>
+        <v>55791231.950221665</v>
       </c>
       <c r="E64">
-        <v>30120344.18809896</v>
+        <v>29838429.274073739</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>67572</v>
+        <v>67937</v>
       </c>
       <c r="B65">
         <v>63.5</v>
       </c>
       <c r="C65">
-        <v>6120724.46</v>
+        <v>6292149.3200000003</v>
       </c>
       <c r="D65">
-        <v>47744568.034139924</v>
+        <v>48159858.818404883</v>
       </c>
       <c r="E65">
-        <v>25491261.917743269</v>
+        <v>25227871.031134009</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>67937</v>
+        <v>68302</v>
       </c>
       <c r="B66">
         <v>64.5</v>
       </c>
       <c r="C66">
-        <v>4553073.71</v>
+        <v>4681602.5999999996</v>
       </c>
       <c r="D66">
-        <v>40901495.523963317</v>
+        <v>41268534.154762141</v>
       </c>
       <c r="E66">
-        <v>21412884.609433409</v>
+        <v>21169250.973493949</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>68302</v>
+        <v>68667</v>
       </c>
       <c r="B67">
         <v>65.5</v>
       </c>
       <c r="C67">
-        <v>3347289.49</v>
+        <v>3442042.69</v>
       </c>
       <c r="D67">
-        <v>34766301.009786725</v>
+        <v>35088009.083248474</v>
       </c>
       <c r="E67">
-        <v>17843594.978496961</v>
+        <v>17620572.402046002</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>68667</v>
+        <v>69033</v>
       </c>
       <c r="B68">
         <v>66.5</v>
       </c>
       <c r="C68">
-        <v>2432744.33</v>
+        <v>2501370.7400000002</v>
       </c>
       <c r="D68">
-        <v>29306437.080577768</v>
+        <v>29585938.246604353</v>
       </c>
       <c r="E68">
-        <v>14742657.851407552</v>
+        <v>14540723.948767908</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>69033</v>
+        <v>69398</v>
       </c>
       <c r="B69">
         <v>67.5</v>
       </c>
       <c r="C69">
-        <v>1752548.29</v>
+        <v>1801365.37</v>
       </c>
       <c r="D69">
-        <v>24486817.612876423</v>
+        <v>24727341.601288818</v>
       </c>
       <c r="E69">
-        <v>12070010.896944989</v>
+        <v>11889269.356152872</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>69398</v>
+        <v>69763</v>
       </c>
       <c r="B70">
         <v>68.5</v>
       </c>
       <c r="C70">
-        <v>1254726.32</v>
+        <v>1288860.3899999999</v>
       </c>
       <c r="D70">
-        <v>20269672.595261738</v>
+        <v>20474491.845707566</v>
       </c>
       <c r="E70">
-        <v>9786430.1858253013</v>
+        <v>9626534.1361398604</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>69763</v>
+        <v>70128</v>
       </c>
       <c r="B71">
         <v>69.5</v>
       </c>
       <c r="C71">
-        <v>898339.49</v>
+        <v>921855.78</v>
       </c>
       <c r="D71">
-        <v>16614284.699550368</v>
+        <v>16786740.768610012</v>
       </c>
       <c r="E71">
-        <v>7853472.2616992518</v>
+        <v>7713663.9164395034</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>70128</v>
+        <v>70494</v>
       </c>
       <c r="B72">
         <v>70.5</v>
       </c>
       <c r="C72">
-        <v>646015.43999999994</v>
+        <v>662042.9</v>
       </c>
       <c r="D72">
-        <v>13477094.061564991</v>
+        <v>13620604.391801871</v>
       </c>
       <c r="E72">
-        <v>6233473.0352941686</v>
+        <v>6112659.9901514407</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>70494</v>
+        <v>70859</v>
       </c>
       <c r="B73">
         <v>71.5</v>
       </c>
       <c r="C73">
-        <v>471257.51</v>
+        <v>482102.5</v>
       </c>
       <c r="D73">
-        <v>10812522.387184499</v>
+        <v>10930497.129484463</v>
       </c>
       <c r="E73">
-        <v>4890039.405112355</v>
+        <v>4786871.5371281961</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>70859</v>
+        <v>71224</v>
       </c>
       <c r="B74">
         <v>72.5</v>
       </c>
       <c r="C74">
-        <v>351379.28</v>
+        <v>358689.48</v>
       </c>
       <c r="D74">
-        <v>8573821.087596124</v>
+        <v>8669542.5472833775</v>
       </c>
       <c r="E74">
-        <v>3788484.8709427943</v>
+        <v>3701449.3464187072</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>71224</v>
+        <v>71589</v>
       </c>
       <c r="B75">
         <v>73.5</v>
       </c>
       <c r="C75">
-        <v>269701.94</v>
+        <v>274637.03000000003</v>
       </c>
       <c r="D75">
-        <v>6713741.8514094828</v>
+        <v>6790276.0898670088</v>
       </c>
       <c r="E75">
-        <v>2896118.3862508121</v>
+        <v>2823622.4151561731</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>71589</v>
+        <v>71955</v>
       </c>
       <c r="B76">
         <v>74.5</v>
       </c>
       <c r="C76">
-        <v>214593.44</v>
+        <v>217960.23</v>
       </c>
       <c r="D76">
-        <v>5186249.9305107808</v>
+        <v>5246397.4382971078</v>
       </c>
       <c r="E76">
-        <v>2182588.4703057469</v>
+        <v>2123037.990304952</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>71955</v>
+        <v>72320</v>
       </c>
       <c r="B77">
         <v>75.5</v>
       </c>
       <c r="C77">
-        <v>176933.39</v>
+        <v>179288.09</v>
       </c>
       <c r="D77">
-        <v>3948189.7343635545</v>
+        <v>3994524.3894720506</v>
       </c>
       <c r="E77">
-        <v>1620102.5713843291</v>
+        <v>1571921.1952047334</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>72320</v>
+        <v>72685</v>
       </c>
       <c r="B78">
         <v>76.5</v>
       </c>
       <c r="C78">
-        <v>150322.99</v>
+        <v>152044.59</v>
       </c>
       <c r="D78">
-        <v>2959046.6048263004</v>
+        <v>2993947.7880517975</v>
       </c>
       <c r="E78">
-        <v>1183429.5575376227</v>
+        <v>1145057.9585733623</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>72685</v>
+        <v>73050</v>
       </c>
       <c r="B79">
         <v>77.5</v>
       </c>
       <c r="C79">
-        <v>130039.49</v>
+        <v>131376.57</v>
       </c>
       <c r="D79">
-        <v>2180927.6856686897</v>
+        <v>2206544.1572660301</v>
       </c>
       <c r="E79">
-        <v>849944.31270371913</v>
+        <v>819894.01799540711</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>73050</v>
+        <v>73415</v>
       </c>
       <c r="B80">
         <v>78.5</v>
       </c>
       <c r="C80">
-        <v>115280.23</v>
+        <v>116384.47</v>
       </c>
       <c r="D80">
-        <v>1579032.9488149334</v>
+        <v>1597268.9566045678</v>
       </c>
       <c r="E80">
-        <v>599674.33110637614</v>
+        <v>576571.23908656347</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>73415</v>
+        <f>+EOMONTH(A80,12)</f>
+        <v>73780</v>
       </c>
       <c r="B81">
         <v>79.5</v>
       </c>
       <c r="C81">
-        <v>103984.81</v>
+        <v>104942.29</v>
       </c>
       <c r="D81">
-        <v>1121814.0427343096</v>
+        <v>1134320.121852173</v>
       </c>
       <c r="E81">
-        <v>415303.93687296356</v>
+        <v>397899.28710025933</v>
       </c>
     </row>
   </sheetData>
@@ -1801,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B07887-8F52-4ACD-9003-CB270BD2655C}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,1362 +1831,1363 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44561</v>
+        <v>44926</v>
       </c>
       <c r="B2">
         <v>0.5</v>
       </c>
       <c r="C2">
-        <v>1511573.39</v>
+        <v>1480324.2242113794</v>
       </c>
       <c r="D2">
-        <v>151550.67918911797</v>
+        <v>151542.48964270126</v>
       </c>
       <c r="E2">
-        <v>856224.83884138486</v>
+        <v>853507.28582016868</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44926</v>
+        <v>45291</v>
       </c>
       <c r="B3">
         <v>1.5</v>
       </c>
       <c r="C3">
-        <v>4341798.12</v>
+        <v>4293848.9963713167</v>
       </c>
       <c r="D3">
-        <v>637883.94351329131</v>
+        <v>637893.46071151469</v>
       </c>
       <c r="E3">
-        <v>3265972.6679074764</v>
+        <v>3257449.0224890145</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45291</v>
+        <v>45657</v>
       </c>
       <c r="B4">
         <v>2.5</v>
       </c>
       <c r="C4">
-        <v>6325185.1100000003</v>
+        <v>6250301.123915934</v>
       </c>
       <c r="D4">
-        <v>1364456.9090522903</v>
+        <v>1364554.9920054036</v>
       </c>
       <c r="E4">
-        <v>6377870.8487443989</v>
+        <v>6362006.883028524</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45657</v>
+        <v>46022</v>
       </c>
       <c r="B5">
         <v>3.5</v>
       </c>
       <c r="C5">
-        <v>8362114.7400000002</v>
+        <v>8255049.3938409537</v>
       </c>
       <c r="D5">
-        <v>2184367.234969791</v>
+        <v>2184632.6095532193</v>
       </c>
       <c r="E5">
-        <v>9520245.220500255</v>
+        <v>9494575.7567297313</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>46022</v>
+        <v>46387</v>
       </c>
       <c r="B6">
         <v>4.5</v>
       </c>
       <c r="C6">
-        <v>10514285.02</v>
+        <v>10381431.015817547</v>
       </c>
       <c r="D6">
-        <v>3091714.3883323232</v>
+        <v>3092235.2306645936</v>
       </c>
       <c r="E6">
-        <v>12717740.88156859</v>
+        <v>12675105.103187175</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>46387</v>
+        <v>46752</v>
       </c>
       <c r="B7">
         <v>5.5</v>
       </c>
       <c r="C7">
-        <v>12623040.98</v>
+        <v>12468679.159448257</v>
       </c>
       <c r="D7">
-        <v>4047642.4320886219</v>
+        <v>4048521.5742307245</v>
       </c>
       <c r="E7">
-        <v>15895660.431755725</v>
+        <v>15830626.075603152</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>46752</v>
+        <v>47118</v>
       </c>
       <c r="B8">
         <v>6.5</v>
       </c>
       <c r="C8">
-        <v>14685498.75</v>
+        <v>14510734.540319595</v>
       </c>
       <c r="D8">
-        <v>5008064.005692088</v>
+        <v>5009412.0818245653</v>
       </c>
       <c r="E8">
-        <v>18972997.307288293</v>
+        <v>18885035.388521247</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>47118</v>
+        <v>47483</v>
       </c>
       <c r="B9">
         <v>7.5</v>
       </c>
       <c r="C9">
-        <v>16613936.24</v>
+        <v>16421348.350879114</v>
       </c>
       <c r="D9">
-        <v>5971958.5223571537</v>
+        <v>5973902.2814260796</v>
       </c>
       <c r="E9">
-        <v>21944840.502876922</v>
+        <v>21832458.516819932</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>47483</v>
+        <v>47848</v>
       </c>
       <c r="B10">
         <v>8.5</v>
       </c>
       <c r="C10">
-        <v>18423386.530000001</v>
+        <v>18213902.233152557</v>
       </c>
       <c r="D10">
-        <v>6928982.9538100325</v>
+        <v>6931660.0427241577</v>
       </c>
       <c r="E10">
-        <v>24819653.988351468</v>
+        <v>24681967.311602328</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>47848</v>
+        <v>48213</v>
       </c>
       <c r="B11">
         <v>9.5</v>
       </c>
       <c r="C11">
-        <v>20212010.289999999</v>
+        <v>19988908.498620246</v>
       </c>
       <c r="D11">
-        <v>7882297.9762343671</v>
+        <v>7885857.5997140491</v>
       </c>
       <c r="E11">
-        <v>27611179.965251222</v>
+        <v>27444356.326740008</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>48213</v>
+        <v>48579</v>
       </c>
       <c r="B12">
         <v>10.5</v>
       </c>
       <c r="C12">
-        <v>21929957.129999999</v>
+        <v>21694750.859167647</v>
       </c>
       <c r="D12">
-        <v>8826003.869571574</v>
+        <v>8830605.4775795564</v>
       </c>
       <c r="E12">
-        <v>30314492.058358438</v>
+        <v>30119575.722258911</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>48579</v>
+        <v>48944</v>
       </c>
       <c r="B13">
         <v>11.5</v>
       </c>
       <c r="C13">
-        <v>23578866.829999998</v>
+        <v>23342197.322482944</v>
       </c>
       <c r="D13">
-        <v>9738667.4972139075</v>
+        <v>9744476.111208722</v>
       </c>
       <c r="E13">
-        <v>32934028.201668572</v>
+        <v>32708480.127799407</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>48944</v>
+        <v>49309</v>
       </c>
       <c r="B14">
         <v>12.5</v>
       </c>
       <c r="C14">
-        <v>25079893.109999999</v>
+        <v>24839304.334838618</v>
       </c>
       <c r="D14">
-        <v>10610528.185557656</v>
+        <v>10617709.88625619</v>
       </c>
       <c r="E14">
-        <v>35449567.981428668</v>
+        <v>35190409.831031986</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>49309</v>
+        <v>49674</v>
       </c>
       <c r="B15">
         <v>13.5</v>
       </c>
       <c r="C15">
-        <v>26403550.949999999</v>
+        <v>26159309.899691425</v>
       </c>
       <c r="D15">
-        <v>11448220.488674341</v>
+        <v>11456942.424841568</v>
       </c>
       <c r="E15">
-        <v>37837366.699690461</v>
+        <v>37541587.01752907</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>49674</v>
+        <v>50040</v>
       </c>
       <c r="B16">
         <v>14.5</v>
       </c>
       <c r="C16">
-        <v>27779064.280000001</v>
+        <v>27541802.855674695</v>
       </c>
       <c r="D16">
-        <v>12252624.576268621</v>
+        <v>12263050.863420643</v>
       </c>
       <c r="E16">
-        <v>40116580.753044814</v>
+        <v>39780960.034711972</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>50040</v>
+        <v>50405</v>
       </c>
       <c r="B17">
         <v>15.5</v>
       </c>
       <c r="C17">
-        <v>28902304.210000001</v>
+        <v>28663625.78265458</v>
       </c>
       <c r="D17">
-        <v>13020632.201723732</v>
+        <v>13032920.820406914</v>
       </c>
       <c r="E17">
-        <v>42309618.348045804</v>
+        <v>41929905.526509926</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>50405</v>
+        <v>50770</v>
       </c>
       <c r="B18">
         <v>16.5</v>
       </c>
       <c r="C18">
-        <v>29852293.030000001</v>
+        <v>29624272.753358331</v>
       </c>
       <c r="D18">
-        <v>13758245.666097505</v>
+        <v>13772547.003720837</v>
       </c>
       <c r="E18">
-        <v>44419338.849225335</v>
+        <v>43991417.091912232</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>50770</v>
+        <v>51135</v>
       </c>
       <c r="B19">
         <v>17.5</v>
       </c>
       <c r="C19">
-        <v>30784820.989999998</v>
+        <v>30571984.938739978</v>
       </c>
       <c r="D19">
-        <v>14466885.601223372</v>
+        <v>14483340.795611482</v>
       </c>
       <c r="E19">
-        <v>46452658.834001057</v>
+        <v>45972334.145702273</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>51135</v>
+        <v>51501</v>
       </c>
       <c r="B20">
         <v>18.5</v>
       </c>
       <c r="C20">
-        <v>31633981.32</v>
+        <v>31449101.197673738</v>
       </c>
       <c r="D20">
-        <v>15162159.539074559</v>
+        <v>15180895.092506493</v>
       </c>
       <c r="E20">
-        <v>48417140.988087013</v>
+        <v>47878551.280887984</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>51501</v>
+        <v>51866</v>
       </c>
       <c r="B21">
         <v>19.5</v>
       </c>
       <c r="C21">
-        <v>32241095.699999999</v>
+        <v>32082190.115630936</v>
       </c>
       <c r="D21">
-        <v>15851555.790506342</v>
+        <v>15872676.626797147</v>
       </c>
       <c r="E21">
-        <v>50297447.620058857</v>
+        <v>49688877.118642777</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>51866</v>
+        <v>52231</v>
       </c>
       <c r="B22">
         <v>20.5</v>
       </c>
       <c r="C22">
-        <v>32620526.489999998</v>
+        <v>32466828.128840819</v>
       </c>
       <c r="D22">
-        <v>16530531.97478848</v>
+        <v>16554119.549562899</v>
       </c>
       <c r="E22">
-        <v>52058150.24131953</v>
+        <v>51370824.041904785</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>52231</v>
+        <v>52596</v>
       </c>
       <c r="B23">
         <v>21.5</v>
       </c>
       <c r="C23">
-        <v>32990196.629999999</v>
+        <v>32863528.714063067</v>
       </c>
       <c r="D23">
-        <v>17204596.515985187</v>
+        <v>17230708.401595533</v>
       </c>
       <c r="E23">
-        <v>53688349.878932402</v>
+        <v>52920128.813968949</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>52596</v>
+        <v>52962</v>
       </c>
       <c r="B24">
         <v>22.5</v>
       </c>
       <c r="C24">
-        <v>33356640.219999999</v>
+        <v>33271445.956951413</v>
       </c>
       <c r="D24">
-        <v>17866721.733866997</v>
+        <v>17895388.289553553</v>
       </c>
       <c r="E24">
-        <v>55217741.262796372</v>
+        <v>54364576.493288949</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>52962</v>
+        <v>53327</v>
       </c>
       <c r="B25">
         <v>23.5</v>
       </c>
       <c r="C25">
-        <v>33476857.629999999</v>
+        <v>33414888.481506739</v>
       </c>
       <c r="D25">
-        <v>18486735.183764592</v>
+        <v>18517954.886238046</v>
       </c>
       <c r="E25">
-        <v>56635739.841628142</v>
+        <v>55690624.237227231</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>53327</v>
+        <v>53692</v>
       </c>
       <c r="B26">
         <v>24.5</v>
       </c>
       <c r="C26">
-        <v>33370512.73</v>
+        <v>33329289.380176775</v>
       </c>
       <c r="D26">
-        <v>19057407.582400095</v>
+        <v>19091146.451081488</v>
       </c>
       <c r="E26">
-        <v>57914594.869739354</v>
+        <v>56870661.085454665</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>53692</v>
+        <v>54057</v>
       </c>
       <c r="B27">
         <v>25.5</v>
       </c>
       <c r="C27">
-        <v>33318724.23</v>
+        <v>33296628.442636512</v>
       </c>
       <c r="D27">
-        <v>19584161.020684991</v>
+        <v>19620356.494179282</v>
       </c>
       <c r="E27">
-        <v>59048553.134188272</v>
+        <v>57901126.505298585</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>54057</v>
+        <v>54423</v>
       </c>
       <c r="B28">
         <v>26.5</v>
       </c>
       <c r="C28">
-        <v>32888777.329999998</v>
+        <v>32909262.32598212</v>
       </c>
       <c r="D28">
-        <v>20055024.041235544</v>
+        <v>20093583.240090195</v>
       </c>
       <c r="E28">
-        <v>60020279.069674917</v>
+        <v>58764914.32565318</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>54423</v>
+        <v>54788</v>
       </c>
       <c r="B29">
         <v>27.5</v>
       </c>
       <c r="C29">
-        <v>32355258.399999999</v>
+        <v>32393279.247077141</v>
       </c>
       <c r="D29">
-        <v>20481645.833987419</v>
+        <v>20522452.530372437</v>
       </c>
       <c r="E29">
-        <v>60835002.340451635</v>
+        <v>59466380.726221606</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>54788</v>
+        <v>55153</v>
       </c>
       <c r="B30">
         <v>28.5</v>
       </c>
       <c r="C30">
-        <v>31523747.91</v>
+        <v>31598504.885900326</v>
       </c>
       <c r="D30">
-        <v>20873771.707106587</v>
+        <v>20916694.573058076</v>
       </c>
       <c r="E30">
-        <v>61484872.696034454</v>
+        <v>59996396.29226508</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>55153</v>
+        <v>55518</v>
       </c>
       <c r="B31">
         <v>29.5</v>
       </c>
       <c r="C31">
-        <v>30317963.27</v>
+        <v>30417478.432316311</v>
       </c>
       <c r="D31">
-        <v>21220547.065165542</v>
+        <v>21265439.918048091</v>
       </c>
       <c r="E31">
-        <v>61933787.671945907</v>
+        <v>60316347.911723316</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>55518</v>
+        <v>55884</v>
       </c>
       <c r="B32">
         <v>30.5</v>
       </c>
       <c r="C32">
-        <v>29225809.300000001</v>
+        <v>29340673.357677847</v>
       </c>
       <c r="D32">
-        <v>21505156.917232614</v>
+        <v>21551864.035802167</v>
       </c>
       <c r="E32">
-        <v>62160449.340626612</v>
+        <v>60408409.542703725</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>55884</v>
+        <v>56249</v>
       </c>
       <c r="B33">
         <v>31.5</v>
       </c>
       <c r="C33">
-        <v>27686081.289999999</v>
+        <v>27821714.537479665</v>
       </c>
       <c r="D33">
-        <v>21726964.934354711</v>
+        <v>21775329.137692936</v>
       </c>
       <c r="E33">
-        <v>62145636.67789869</v>
+        <v>60260587.801319174</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>56249</v>
+        <v>56614</v>
       </c>
       <c r="B34">
         <v>32.5</v>
       </c>
       <c r="C34">
-        <v>26085189.039999999</v>
+        <v>26238701.977424517</v>
       </c>
       <c r="D34">
-        <v>21921741.603587955</v>
+        <v>21971608.712901954</v>
       </c>
       <c r="E34">
-        <v>61884189.313082024</v>
+        <v>59872939.297520421</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>56614</v>
+        <v>56979</v>
       </c>
       <c r="B35">
         <v>33.5</v>
       </c>
       <c r="C35">
-        <v>24380986.760000002</v>
+        <v>24550017.743211832</v>
       </c>
       <c r="D35">
-        <v>22105730.096118517</v>
+        <v>22156949.770969369</v>
       </c>
       <c r="E35">
-        <v>61369835.814161554</v>
+        <v>59238695.265142344</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>56979</v>
+        <v>57345</v>
       </c>
       <c r="B36">
         <v>34.5</v>
       </c>
       <c r="C36">
-        <v>22602112.75</v>
+        <v>22782570.624601971</v>
       </c>
       <c r="D36">
-        <v>22281297.768135577</v>
+        <v>22333728.214657489</v>
       </c>
       <c r="E36">
-        <v>60598694.432418928</v>
+        <v>58351544.334336862</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>57345</v>
+        <v>57710</v>
       </c>
       <c r="B37">
         <v>35.5</v>
       </c>
       <c r="C37">
-        <v>20892990.940000001</v>
+        <v>21084668.523620632</v>
       </c>
       <c r="D37">
-        <v>22449316.365530454</v>
+        <v>22502829.569036476</v>
       </c>
       <c r="E37">
-        <v>59578862.588664576</v>
+        <v>57220748.625263482</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>57710</v>
+        <v>58075</v>
       </c>
       <c r="B38">
         <v>36.5</v>
       </c>
       <c r="C38">
-        <v>19310022.140000001</v>
+        <v>19508019.708151761</v>
       </c>
       <c r="D38">
-        <v>22624245.769705147</v>
+        <v>22678729.438879482</v>
       </c>
       <c r="E38">
-        <v>58278569.136181265</v>
+        <v>55828758.66093234</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>58075</v>
+        <v>58440</v>
       </c>
       <c r="B39">
         <v>37.5</v>
       </c>
       <c r="C39">
-        <v>17920127.460000001</v>
+        <v>18132405.468249068</v>
       </c>
       <c r="D39">
-        <v>22841175.057487961</v>
+        <v>22896535.992083035</v>
       </c>
       <c r="E39">
-        <v>56699939.329380855</v>
+        <v>54196650.311278656</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>58440</v>
+        <v>58806</v>
       </c>
       <c r="B40">
         <v>38.5</v>
       </c>
       <c r="C40">
-        <v>16539254.01</v>
+        <v>16755665.273748156</v>
       </c>
       <c r="D40">
-        <v>23071828.080248237</v>
+        <v>23127980.753175564</v>
       </c>
       <c r="E40">
-        <v>54928106.501201212</v>
+        <v>52397224.67017214</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>58806</v>
+        <v>59171</v>
       </c>
       <c r="B41">
         <v>39.5</v>
       </c>
       <c r="C41">
-        <v>15206093.33</v>
+        <v>15426787.591633705</v>
       </c>
       <c r="D41">
-        <v>23069326.211545404</v>
+        <v>23126147.8848808</v>
       </c>
       <c r="E41">
-        <v>53024812.94409024</v>
+        <v>50476353.423770569</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>59171</v>
+        <v>59536</v>
       </c>
       <c r="B42">
         <v>40.5</v>
       </c>
       <c r="C42">
-        <v>13924016.82</v>
+        <v>14145876.529691121</v>
       </c>
       <c r="D42">
-        <v>22811044.034645889</v>
+        <v>22868412.228984956</v>
       </c>
       <c r="E42">
-        <v>51007356.393629044</v>
+        <v>48451544.969263151</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>59536</v>
+        <v>59901</v>
       </c>
       <c r="B43">
         <v>41.5</v>
       </c>
       <c r="C43">
-        <v>12698003.640000001</v>
+        <v>12919852.84271335</v>
       </c>
       <c r="D43">
-        <v>22566925.884452429</v>
+        <v>22624779.604495782</v>
       </c>
       <c r="E43">
-        <v>48888892.513533987</v>
+        <v>46340765.000131123</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>59901</v>
+        <v>60267</v>
       </c>
       <c r="B44">
         <v>42.5</v>
       </c>
       <c r="C44">
-        <v>11531056.050000001</v>
+        <v>11750814.934607655</v>
       </c>
       <c r="D44">
-        <v>22436595.261635289</v>
+        <v>22494908.318431042</v>
       </c>
       <c r="E44">
-        <v>46694830.354483202</v>
+        <v>44172335.55584649</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>60267</v>
+        <v>60632</v>
       </c>
       <c r="B45">
         <v>43.5</v>
       </c>
       <c r="C45">
-        <v>10423882.109999999</v>
+        <v>10639766.985764632</v>
       </c>
       <c r="D45">
-        <v>22114047.479760662</v>
+        <v>22172745.674838468</v>
       </c>
       <c r="E45">
-        <v>44458492.934551671</v>
+        <v>41975845.765347295</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>60632</v>
+        <v>60997</v>
       </c>
       <c r="B46">
         <v>44.5</v>
       </c>
       <c r="C46">
-        <v>9376590.3900000006</v>
+        <v>9586917.3109616376</v>
       </c>
       <c r="D46">
-        <v>21383633.301057655</v>
+        <v>21442606.083639815</v>
       </c>
       <c r="E46">
-        <v>42206456.591490991</v>
+        <v>39774557.724725142</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>60997</v>
+        <v>61362</v>
       </c>
       <c r="B47">
         <v>45.5</v>
       </c>
       <c r="C47">
-        <v>8391263.4600000009</v>
+        <v>8594509.4848421384</v>
       </c>
       <c r="D47">
-        <v>20501766.220901571</v>
+        <v>20560953.138471838</v>
       </c>
       <c r="E47">
-        <v>39959797.262861319</v>
+        <v>37587076.486660495</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>61362</v>
+        <v>61728</v>
       </c>
       <c r="B48">
         <v>46.5</v>
       </c>
       <c r="C48">
-        <v>7469421.4500000002</v>
+        <v>7664257.3635288971</v>
       </c>
       <c r="D48">
-        <v>19619193.862178568</v>
+        <v>19678556.509796891</v>
       </c>
       <c r="E48">
-        <v>37733641.341273293</v>
+        <v>35426194.380697556</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>61728</v>
+        <v>62093</v>
       </c>
       <c r="B49">
         <v>47.5</v>
       </c>
       <c r="C49">
-        <v>6609971.1500000004</v>
+        <v>6795249.3375787586</v>
       </c>
       <c r="D49">
-        <v>18737147.250226244</v>
+        <v>18796646.730154343</v>
       </c>
       <c r="E49">
-        <v>35538188.605197527</v>
+        <v>33300674.862129819</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>62093</v>
+        <v>62458</v>
       </c>
       <c r="B50">
         <v>48.5</v>
       </c>
       <c r="C50">
-        <v>5813554.6600000001</v>
+        <v>5988315.8038331578</v>
       </c>
       <c r="D50">
-        <v>17856213.207779586</v>
+        <v>17915803.031242851</v>
       </c>
       <c r="E50">
-        <v>33377559.18710709</v>
+        <v>31215161.836576086</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>62458</v>
+        <v>62823</v>
       </c>
       <c r="B51">
         <v>49.5</v>
       </c>
       <c r="C51">
-        <v>5080046.17</v>
+        <v>5243532.875479023</v>
       </c>
       <c r="D51">
-        <v>16977535.78512634</v>
+        <v>17037154.293036271</v>
       </c>
       <c r="E51">
-        <v>31257909.085107982</v>
+        <v>29176454.786744218</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>62823</v>
+        <v>63189</v>
       </c>
       <c r="B52">
         <v>50.5</v>
       </c>
       <c r="C52">
-        <v>4408739.8899999997</v>
+        <v>4560402.3294574358</v>
       </c>
       <c r="D52">
-        <v>16103050.755559592</v>
+        <v>16162614.783221126</v>
       </c>
       <c r="E52">
-        <v>29189990.523792841</v>
+        <v>27193199.561300345</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>63189</v>
+        <v>63554</v>
       </c>
       <c r="B53">
         <v>51.5</v>
       </c>
       <c r="C53">
-        <v>3798385.72</v>
+        <v>3937869.7548964536</v>
       </c>
       <c r="D53">
-        <v>15234180.792275734</v>
+        <v>15293580.748972112</v>
       </c>
       <c r="E53">
-        <v>27180269.324777618</v>
+        <v>25270062.080512874</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>63554</v>
+        <v>63919</v>
       </c>
       <c r="B54">
         <v>52.5</v>
       </c>
       <c r="C54">
-        <v>3247315.41</v>
+        <v>3374463.1535093179</v>
       </c>
       <c r="D54">
-        <v>14372165.482625157</v>
+        <v>14431269.700461941</v>
       </c>
       <c r="E54">
-        <v>25230488.754697539</v>
+        <v>23408630.367384732</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>63919</v>
+        <v>64284</v>
       </c>
       <c r="B55">
         <v>53.5</v>
       </c>
       <c r="C55">
-        <v>2753453.18</v>
+        <v>2868292.1742316415</v>
       </c>
       <c r="D55">
-        <v>13518364.425870856</v>
+        <v>13577025.786435066</v>
       </c>
       <c r="E55">
-        <v>23342641.665142179</v>
+        <v>21610641.685887225</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>64284</v>
+        <v>64650</v>
       </c>
       <c r="B56">
         <v>54.5</v>
       </c>
       <c r="C56">
-        <v>2314355.85</v>
+        <v>2417084.1653964114</v>
       </c>
       <c r="D56">
-        <v>12674266.750256039</v>
+        <v>12732317.709305668</v>
       </c>
       <c r="E56">
-        <v>21518684.54423755</v>
+        <v>19877734.39074285</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>64650</v>
+        <v>65015</v>
       </c>
       <c r="B57">
         <v>55.5</v>
       </c>
       <c r="C57">
-        <v>1927233.29</v>
+        <v>2018206.8440550747</v>
       </c>
       <c r="D57">
-        <v>11841524.074230764</v>
+        <v>11898771.699779557</v>
       </c>
       <c r="E57">
-        <v>19760368.323634773</v>
+        <v>18211438.843848299</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>65015</v>
+        <v>65380</v>
       </c>
       <c r="B58">
         <v>56.5</v>
       </c>
       <c r="C58">
-        <v>1589012.43</v>
+        <v>1668729.3971972333</v>
       </c>
       <c r="D58">
-        <v>11021917.865781751</v>
+        <v>11078149.119256608</v>
       </c>
       <c r="E58">
-        <v>18069619.968383577</v>
+        <v>16613456.139895046</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>65380</v>
+        <v>65745</v>
       </c>
       <c r="B59">
         <v>57.5</v>
       </c>
       <c r="C59">
-        <v>1296379.9099999999</v>
+        <v>1365457.5302280213</v>
       </c>
       <c r="D59">
-        <v>10217344.118804824</v>
+        <v>10272330.594848743</v>
       </c>
       <c r="E59">
-        <v>16448661.844543574</v>
+        <v>15085669.45342824</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>65745</v>
+        <v>66111</v>
       </c>
       <c r="B60">
         <v>58.5</v>
       </c>
       <c r="C60">
-        <v>1045839.02</v>
+        <v>1105002.8512951622</v>
       </c>
       <c r="D60">
-        <v>9429841.4587285202</v>
+        <v>9483344.2336123362</v>
       </c>
       <c r="E60">
-        <v>14899859.105486147</v>
+        <v>13630066.005969351</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>66111</v>
+        <v>66476</v>
       </c>
       <c r="B61">
         <v>59.5</v>
       </c>
       <c r="C61">
-        <v>833743.02</v>
+        <v>883802.81156533805</v>
       </c>
       <c r="D61">
-        <v>8661575.9941969384</v>
+        <v>8713352.3920996934</v>
       </c>
       <c r="E61">
-        <v>13425607.032663845</v>
+        <v>12248632.918981988</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>66476</v>
+        <v>66841</v>
       </c>
       <c r="B62">
         <v>60.5</v>
       </c>
       <c r="C62">
-        <v>656330.35</v>
+        <v>698145.4951142926</v>
       </c>
       <c r="D62">
-        <v>7914806.3975663185</v>
+        <v>7964614.8022643244</v>
       </c>
       <c r="E62">
-        <v>12028270.028456362</v>
+        <v>10943296.157121336</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>66841</v>
+        <v>67206</v>
       </c>
       <c r="B63">
         <v>61.5</v>
       </c>
       <c r="C63">
-        <v>509823.23</v>
+        <v>544275.02626118413</v>
       </c>
       <c r="D63">
-        <v>7191822.7156260135</v>
+        <v>7239428.0390322534</v>
       </c>
       <c r="E63">
-        <v>10710184.08484384</v>
+        <v>9715927.320641119</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>67206</v>
+        <v>67572</v>
       </c>
       <c r="B64">
         <v>62.5</v>
       </c>
       <c r="C64">
-        <v>390478.88</v>
+        <v>418457.96356672799</v>
       </c>
       <c r="D64">
-        <v>6494939.4689640198</v>
+        <v>6540117.3703037761</v>
       </c>
       <c r="E64">
-        <v>9473482.0118292961</v>
+        <v>8568177.0788843464</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>67572</v>
+        <v>67937</v>
       </c>
       <c r="B65">
         <v>63.5</v>
       </c>
       <c r="C65">
-        <v>294668.92</v>
+        <v>317052.97833790135</v>
       </c>
       <c r="D65">
-        <v>5826491.4124948159</v>
+        <v>5869035.2739286441</v>
       </c>
       <c r="E65">
-        <v>8319986.4646641342</v>
+        <v>7501367.6877569137</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>67937</v>
+        <v>68302</v>
       </c>
       <c r="B66">
         <v>64.5</v>
       </c>
       <c r="C66">
-        <v>218940.5</v>
+        <v>236575.38231801955</v>
       </c>
       <c r="D66">
-        <v>5188841.542723543</v>
+        <v>5228575.3997172499</v>
       </c>
       <c r="E66">
-        <v>7251103.3733937545</v>
+        <v>6516411.0252691954</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>68302</v>
+        <v>68667</v>
       </c>
       <c r="B67">
         <v>65.5</v>
       </c>
       <c r="C67">
-        <v>160056.79</v>
+        <v>173731.67822681615</v>
       </c>
       <c r="D67">
-        <v>4584419.631890187</v>
+        <v>4621203.2402388593</v>
       </c>
       <c r="E67">
-        <v>6267772.6665007202</v>
+        <v>5613737.3731370121</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>68667</v>
+        <v>69033</v>
       </c>
       <c r="B68">
         <v>66.5</v>
       </c>
       <c r="C68">
-        <v>115053.15</v>
+        <v>125482.18286134882</v>
       </c>
       <c r="D68">
-        <v>4015648.2848638208</v>
+        <v>4049378.8044801741</v>
       </c>
       <c r="E68">
-        <v>5370329.3656590926</v>
+        <v>4793181.7741595935</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>69033</v>
+        <v>69398</v>
       </c>
       <c r="B69">
         <v>67.5</v>
       </c>
       <c r="C69">
-        <v>81269</v>
+        <v>89088.003080575509</v>
       </c>
       <c r="D69">
-        <v>3484928.2436723537</v>
+        <v>3515540.9959954969</v>
       </c>
       <c r="E69">
-        <v>4558419.1666293917</v>
+        <v>4053910.0508217267</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>69398</v>
+        <v>69763</v>
       </c>
       <c r="B70">
         <v>68.5</v>
       </c>
       <c r="C70">
-        <v>56374.66</v>
+        <v>62136.872388721065</v>
       </c>
       <c r="D70">
-        <v>2994548.4359521107</v>
+        <v>3022020.7388938004</v>
       </c>
       <c r="E70">
-        <v>3830951.6493350849</v>
+        <v>3394354.6205073437</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>69763</v>
+        <v>70128</v>
       </c>
       <c r="B71">
         <v>69.5</v>
       </c>
       <c r="C71">
-        <v>38383.07</v>
+        <v>42556.714626449655</v>
       </c>
       <c r="D71">
-        <v>2546367.4709542468</v>
+        <v>2570728.7250806666</v>
       </c>
       <c r="E71">
-        <v>3185920.6065888861</v>
+        <v>2812082.5552139655</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>70128</v>
+        <v>70494</v>
       </c>
       <c r="B72">
         <v>70.5</v>
       </c>
       <c r="C72">
-        <v>25637.97</v>
+        <v>28609.924424328488</v>
       </c>
       <c r="D72">
-        <v>2141498.292569722</v>
+        <v>2162832.4570665834</v>
       </c>
       <c r="E72">
-        <v>2620273.2342246012</v>
+        <v>2303717.901747026</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>70494</v>
+        <v>70859</v>
       </c>
       <c r="B73">
         <v>71.5</v>
       </c>
       <c r="C73">
-        <v>16794.060000000001</v>
+        <v>18873.381049655458</v>
       </c>
       <c r="D73">
-        <v>1780193.6856725751</v>
+        <v>1798632.0951283562</v>
       </c>
       <c r="E73">
-        <v>2129959.0366377993</v>
+        <v>1865008.7193233322</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>70859</v>
+        <v>71224</v>
       </c>
       <c r="B74">
         <v>72.5</v>
       </c>
       <c r="C74">
-        <v>10785.59</v>
+        <v>12213.693350672356</v>
       </c>
       <c r="D74">
-        <v>1461809.6506789234</v>
+        <v>1477520.2429071274</v>
       </c>
       <c r="E74">
-        <v>1710059.6024620859</v>
+        <v>1490976.663464851</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>71224</v>
+        <v>71589</v>
       </c>
       <c r="B75">
         <v>73.5</v>
       </c>
       <c r="C75">
-        <v>6789.95</v>
+        <v>7751.6989021656518</v>
       </c>
       <c r="D75">
-        <v>1184735.6696787814</v>
+        <v>1197914.201882445</v>
       </c>
       <c r="E75">
-        <v>1354922.08139398</v>
+        <v>1176068.601249408</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>71589</v>
+        <v>71955</v>
       </c>
       <c r="B76">
         <v>74.5</v>
       </c>
       <c r="C76">
-        <v>4189.92</v>
+        <v>4824.361586256573</v>
       </c>
       <c r="D76">
-        <v>946622.80839120026</v>
+        <v>957483.25418627926</v>
       </c>
       <c r="E76">
-        <v>1058439.3826688631</v>
+        <v>914425.98314517189</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>71955</v>
+        <v>72320</v>
       </c>
       <c r="B77">
         <v>75.5</v>
       </c>
       <c r="C77">
-        <v>2534.2399999999998</v>
+        <v>2944.1059782446609</v>
       </c>
       <c r="D77">
-        <v>744836.81196202256</v>
+        <v>753608.50839756418</v>
       </c>
       <c r="E77">
-        <v>814400.45947840484</v>
+        <v>700152.25580501626</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>72320</v>
+        <v>72685</v>
       </c>
       <c r="B78">
         <v>76.5</v>
       </c>
       <c r="C78">
-        <v>1502.48</v>
+        <v>1762.0322934518504</v>
       </c>
       <c r="D78">
-        <v>576505.32318642561</v>
+        <v>583431.76099079091</v>
       </c>
       <c r="E78">
-        <v>616616.40525432571</v>
+        <v>527400.94828807283</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>72685</v>
+        <v>73050</v>
       </c>
       <c r="B79">
         <v>77.5</v>
       </c>
       <c r="C79">
-        <v>873.21</v>
+        <v>1034.4438227360313</v>
       </c>
       <c r="D79">
-        <v>438445.52291485667</v>
+        <v>443774.07097124361</v>
       </c>
       <c r="E79">
-        <v>458945.74127248098</v>
+        <v>390438.00132461288</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>73050</v>
+        <v>73415</v>
       </c>
       <c r="B80">
         <v>78.5</v>
       </c>
       <c r="C80">
-        <v>497.56</v>
+        <v>595.86459984165424</v>
       </c>
       <c r="D80">
-        <v>327267.58886365755</v>
+        <v>331239.29571562022</v>
       </c>
       <c r="E80">
-        <v>335463.24118852225</v>
+        <v>283781.92345908063</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>73415</v>
+        <f>+EOMONTH(A80,12)</f>
+        <v>73780</v>
       </c>
       <c r="B81">
         <v>79.5</v>
       </c>
       <c r="C81">
-        <v>278.02999999999997</v>
+        <v>336.86952569318998</v>
       </c>
       <c r="D81">
-        <v>239482.30715700804</v>
+        <v>242323.40159447814</v>
       </c>
       <c r="E81">
-        <v>240563.79554153321</v>
+        <v>202299.55102132255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data to include total plan
</commit_message>
<xml_diff>
--- a/data/time_series/annual_cashflows_data.xlsx
+++ b/data/time_series/annual_cashflows_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\UPS_MV\data\time_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2C8723-B80B-4580-81DE-6784E4A9592A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C54F7A-6559-4C96-8031-0C8D3F487BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="1260" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{F3CCDB8E-F5F3-42E2-A382-F3745238F716}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3CCDB8E-F5F3-42E2-A382-F3745238F716}"/>
   </bookViews>
   <sheets>
     <sheet name="PBO" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="6">
   <si>
     <t>Time</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -403,19 +406,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027456B0-4AAC-4E49-B406-E9435788ACC8}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A81"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -431,8 +435,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44926</v>
       </c>
@@ -448,8 +455,12 @@
       <c r="E2">
         <v>424015774.05129546</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>SUM(C2:E2)</f>
+        <v>1900302161.589886</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45291</v>
       </c>
@@ -465,8 +476,12 @@
       <c r="E3">
         <v>457065275.86267245</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">SUM(C3:E3)</f>
+        <v>2020151763.154635</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45657</v>
       </c>
@@ -482,8 +497,12 @@
       <c r="E4">
         <v>488405515.40864128</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>2143289539.6888652</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>46022</v>
       </c>
@@ -499,8 +518,12 @@
       <c r="E5">
         <v>516863212.12272674</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>2263219280.6844535</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>46387</v>
       </c>
@@ -516,8 +539,12 @@
       <c r="E6">
         <v>540963075.93295217</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>2378229922.7202206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>46752</v>
       </c>
@@ -533,8 +560,12 @@
       <c r="E7">
         <v>563238770.2817446</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>2487809416.7291493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>47118</v>
       </c>
@@ -550,8 +581,12 @@
       <c r="E8">
         <v>583346925.73878193</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2588719986.4723053</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>47483</v>
       </c>
@@ -567,8 +602,12 @@
       <c r="E9">
         <v>600262968.05763745</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>2676643621.5606418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>47848</v>
       </c>
@@ -584,8 +623,12 @@
       <c r="E10">
         <v>614431256.93380749</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>2755264883.4379897</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>48213</v>
       </c>
@@ -601,8 +644,12 @@
       <c r="E11">
         <v>626399997.06846392</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>2826271040.1890206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>48579</v>
       </c>
@@ -618,8 +665,12 @@
       <c r="E12">
         <v>637224083.46310794</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>2888271473.4495025</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>48944</v>
       </c>
@@ -635,8 +686,12 @@
       <c r="E13">
         <v>646549908.19188178</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>2939701384.4505935</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>49309</v>
       </c>
@@ -652,8 +707,12 @@
       <c r="E14">
         <v>654004643.88014925</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>2979107328.0932202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>49674</v>
       </c>
@@ -669,8 +728,12 @@
       <c r="E15">
         <v>659341735.95668685</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>3004409353.6803422</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>50040</v>
       </c>
@@ -686,8 +749,12 @@
       <c r="E16">
         <v>663292666.11693799</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>3021306495.7408395</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>50405</v>
       </c>
@@ -703,8 +770,12 @@
       <c r="E17">
         <v>667565374.02980375</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>3028896689.7751517</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>50770</v>
       </c>
@@ -720,8 +791,12 @@
       <c r="E18">
         <v>672200031.14548743</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>3028778936.1405005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>51135</v>
       </c>
@@ -737,8 +812,12 @@
       <c r="E19">
         <v>675957099.92138398</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>3020278869.5653458</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>51501</v>
       </c>
@@ -754,8 +833,12 @@
       <c r="E20">
         <v>678178758.23305225</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>3004450910.2089643</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>51866</v>
       </c>
@@ -771,8 +854,12 @@
       <c r="E21">
         <v>678671493.26447356</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>2978605659.7186956</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>52231</v>
       </c>
@@ -788,8 +875,12 @@
       <c r="E22">
         <v>677334354.24249148</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>2946491311.5633831</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>52596</v>
       </c>
@@ -805,8 +896,12 @@
       <c r="E23">
         <v>674115982.06267798</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>2906705196.4478106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>52962</v>
       </c>
@@ -822,8 +917,12 @@
       <c r="E24">
         <v>669200470.54096711</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>2861470690.0765162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>53327</v>
       </c>
@@ -839,8 +938,12 @@
       <c r="E25">
         <v>662461057.13785613</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>2806430331.0220728</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>53692</v>
       </c>
@@ -856,8 +959,12 @@
       <c r="E26">
         <v>653748623.38036883</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>2742611174.2693844</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>54057</v>
       </c>
@@ -873,8 +980,12 @@
       <c r="E27">
         <v>643184810.84966457</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>2672486080.9824295</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>54423</v>
       </c>
@@ -890,8 +1001,12 @@
       <c r="E28">
         <v>630714294.71687984</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>2594602345.0004911</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>54788</v>
       </c>
@@ -907,8 +1022,12 @@
       <c r="E29">
         <v>616448234.49187398</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>2509351816.4895716</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>55153</v>
       </c>
@@ -924,8 +1043,12 @@
       <c r="E30">
         <v>600573880.64061856</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>2416844711.3596849</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>55518</v>
       </c>
@@ -941,8 +1064,12 @@
       <c r="E31">
         <v>588969020.39382529</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>2321699509.3873577</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>55884</v>
       </c>
@@ -958,8 +1085,12 @@
       <c r="E32">
         <v>654617847.92331505</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>2302194352.0016174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>56249</v>
       </c>
@@ -975,8 +1106,12 @@
       <c r="E33">
         <v>700458249.75067556</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>2257259567.8007245</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>56614</v>
       </c>
@@ -992,8 +1127,12 @@
       <c r="E34">
         <v>661931725.8571496</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>2127827052.7449222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>56979</v>
       </c>
@@ -1009,8 +1148,12 @@
       <c r="E35">
         <v>622775801.94075274</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>1998999094.9463575</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>57345</v>
       </c>
@@ -1026,8 +1169,12 @@
       <c r="E36">
         <v>583337433.7355845</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>1870390178.0264375</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>57710</v>
       </c>
@@ -1043,8 +1190,12 @@
       <c r="E37">
         <v>550942897.15521514</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>1750974574.8029785</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>58075</v>
       </c>
@@ -1060,8 +1211,12 @@
       <c r="E38">
         <v>520626161.2241593</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>1637593573.6520066</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>58440</v>
       </c>
@@ -1077,8 +1232,12 @@
       <c r="E39">
         <v>484646188.42140341</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>1522567272.034066</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>58806</v>
       </c>
@@ -1094,8 +1253,12 @@
       <c r="E40">
         <v>449628286.54489565</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>1411714628.9796789</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>59171</v>
       </c>
@@ -1111,8 +1274,12 @@
       <c r="E41">
         <v>415783852.15479821</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>1305209582.2235873</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>59536</v>
       </c>
@@ -1128,8 +1295,12 @@
       <c r="E42">
         <v>383281984.03516048</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>1203291788.1824179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>59901</v>
       </c>
@@ -1145,8 +1316,12 @@
       <c r="E43">
         <v>352252008.24275076</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>1106926314.1439695</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>60267</v>
       </c>
@@ -1162,8 +1337,12 @@
       <c r="E44">
         <v>322811822.83203197</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>1016281950.9691743</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>60632</v>
       </c>
@@ -1179,8 +1358,12 @@
       <c r="E45">
         <v>295036481.24885195</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>929940606.88994575</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>60997</v>
       </c>
@@ -1196,8 +1379,12 @@
       <c r="E46">
         <v>268953117.07541275</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>847694226.98008454</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>61362</v>
       </c>
@@ -1213,8 +1400,12 @@
       <c r="E47">
         <v>244555347.35137379</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>770804595.82971752</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>61728</v>
       </c>
@@ -1230,8 +1421,12 @@
       <c r="E48">
         <v>221813807.83115515</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>699229443.73585749</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>62093</v>
       </c>
@@ -1247,8 +1442,12 @@
       <c r="E49">
         <v>200684753.11110151</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>632751634.47327268</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>62458</v>
       </c>
@@ -1264,8 +1463,12 @@
       <c r="E50">
         <v>181108394.59670976</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>571140144.00146842</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>62823</v>
       </c>
@@ -1281,8 +1484,12 @@
       <c r="E51">
         <v>163019465.61501855</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>514159167.11260045</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>63189</v>
       </c>
@@ -1298,8 +1505,12 @@
       <c r="E52">
         <v>146345463.57891101</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>461566722.77587968</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>63554</v>
       </c>
@@ -1315,8 +1526,12 @@
       <c r="E53">
         <v>131006499.70167373</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>413117658.15170074</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>63919</v>
       </c>
@@ -1332,8 +1547,12 @@
       <c r="E54">
         <v>116922505.81858487</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>368577453.96095121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>64284</v>
       </c>
@@ -1349,8 +1568,12 @@
       <c r="E55">
         <v>104016625.59105338</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>327724642.64516091</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>64650</v>
       </c>
@@ -1366,8 +1589,12 @@
       <c r="E56">
         <v>92214859.748915792</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>290348750.42843556</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>65015</v>
       </c>
@@ -1383,8 +1610,12 @@
       <c r="E57">
         <v>81446613.403591797</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>256249344.638933</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>65380</v>
       </c>
@@ -1400,8 +1631,12 @@
       <c r="E58">
         <v>71642420.750188708</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>225232188.71205539</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>65745</v>
       </c>
@@ -1417,8 +1652,12 @@
       <c r="E59">
         <v>62743807.462651148</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>197117084.45253736</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>66111</v>
       </c>
@@ -1434,8 +1673,12 @@
       <c r="E60">
         <v>54688813.412922546</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>171724032.88891357</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>66476</v>
       </c>
@@ -1451,8 +1694,12 @@
       <c r="E61">
         <v>47421568.635305598</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>148881286.56306124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>66841</v>
       </c>
@@ -1468,8 +1715,12 @@
       <c r="E62">
         <v>40889651.017982721</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>128419109.78417496</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>67206</v>
       </c>
@@ -1485,8 +1736,12 @@
       <c r="E63">
         <v>35044137.800875515</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>110172137.70422076</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>67572</v>
       </c>
@@ -1502,8 +1757,12 @@
       <c r="E64">
         <v>29838429.274073739</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>93979130.014295399</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>67937</v>
       </c>
@@ -1519,8 +1778,12 @@
       <c r="E65">
         <v>25227871.031134009</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>79679879.169538885</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>68302</v>
       </c>
@@ -1536,8 +1799,12 @@
       <c r="E66">
         <v>21169250.973493949</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>67119387.728256091</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>68667</v>
       </c>
@@ -1553,8 +1820,12 @@
       <c r="E67">
         <v>17620572.402046002</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <f t="shared" ref="F67:F81" si="1">SUM(C67:E67)</f>
+        <v>56150624.175294474</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>69033</v>
       </c>
@@ -1570,8 +1841,12 @@
       <c r="E68">
         <v>14540723.948767908</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>46628032.935372263</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>69398</v>
       </c>
@@ -1587,8 +1862,12 @@
       <c r="E69">
         <v>11889269.356152872</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>38417976.327441692</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69763</v>
       </c>
@@ -1604,8 +1883,12 @@
       <c r="E70">
         <v>9626534.1361398604</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>31389886.371847428</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70128</v>
       </c>
@@ -1621,8 +1904,12 @@
       <c r="E71">
         <v>7713663.9164395034</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>25422260.465049516</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70494</v>
       </c>
@@ -1638,8 +1925,12 @@
       <c r="E72">
         <v>6112659.9901514407</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>20395307.281953312</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>70859</v>
       </c>
@@ -1655,8 +1946,12 @@
       <c r="E73">
         <v>4786871.5371281961</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>16199471.166612659</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>71224</v>
       </c>
@@ -1672,8 +1967,12 @@
       <c r="E74">
         <v>3701449.3464187072</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>12729681.373702085</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>71589</v>
       </c>
@@ -1689,8 +1988,12 @@
       <c r="E75">
         <v>2823622.4151561731</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>9888535.5350231826</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>71955</v>
       </c>
@@ -1706,8 +2009,12 @@
       <c r="E76">
         <v>2123037.990304952</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>7587395.6586020608</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>72320</v>
       </c>
@@ -1723,8 +2030,12 @@
       <c r="E77">
         <v>1571921.1952047334</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>5745733.6746767834</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>72685</v>
       </c>
@@ -1740,8 +2051,12 @@
       <c r="E78">
         <v>1145057.9585733623</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>4291050.3366251597</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>73050</v>
       </c>
@@ -1757,8 +2072,12 @@
       <c r="E79">
         <v>819894.01799540711</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>3157814.7452614373</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>73415</v>
       </c>
@@ -1774,8 +2093,12 @@
       <c r="E80">
         <v>576571.23908656347</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>2290224.6656911313</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f>+EOMONTH(A80,12)</f>
         <v>73780</v>
@@ -1791,6 +2114,10 @@
       </c>
       <c r="E81">
         <v>397899.28710025933</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>1637161.6989524323</v>
       </c>
     </row>
   </sheetData>
@@ -1800,10 +2127,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B07887-8F52-4ACD-9003-CB270BD2655C}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E81"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,7 +2139,7 @@
     <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1828,8 +2155,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44926</v>
       </c>
@@ -1845,8 +2175,12 @@
       <c r="E2">
         <v>853507.28582016868</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>SUM(C2:E2)</f>
+        <v>2485373.9996742494</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45291</v>
       </c>
@@ -1862,8 +2196,12 @@
       <c r="E3">
         <v>3257449.0224890145</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">SUM(C3:E3)</f>
+        <v>8189191.4795718454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45657</v>
       </c>
@@ -1879,8 +2217,12 @@
       <c r="E4">
         <v>6362006.883028524</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>13976862.998949861</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>46022</v>
       </c>
@@ -1896,8 +2238,12 @@
       <c r="E5">
         <v>9494575.7567297313</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>19934257.760123905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>46387</v>
       </c>
@@ -1913,8 +2259,12 @@
       <c r="E6">
         <v>12675105.103187175</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>26148771.349669315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>46752</v>
       </c>
@@ -1930,8 +2280,12 @@
       <c r="E7">
         <v>15830626.075603152</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>32347826.809282131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>47118</v>
       </c>
@@ -1947,8 +2301,12 @@
       <c r="E8">
         <v>18885035.388521247</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>38405182.010665409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>47483</v>
       </c>
@@ -1964,8 +2322,12 @@
       <c r="E9">
         <v>21832458.516819932</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>44227709.149125129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>47848</v>
       </c>
@@ -1981,8 +2343,12 @@
       <c r="E10">
         <v>24681967.311602328</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>49827529.58747904</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>48213</v>
       </c>
@@ -1998,8 +2364,12 @@
       <c r="E11">
         <v>27444356.326740008</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>55319122.425074302</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>48579</v>
       </c>
@@ -2015,8 +2385,12 @@
       <c r="E12">
         <v>30119575.722258911</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>60644932.05900611</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>48944</v>
       </c>
@@ -2032,8 +2406,12 @@
       <c r="E13">
         <v>32708480.127799407</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>65795153.561491072</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>49309</v>
       </c>
@@ -2049,8 +2427,12 @@
       <c r="E14">
         <v>35190409.831031986</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>70647424.052126795</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>49674</v>
       </c>
@@ -2066,8 +2448,12 @@
       <c r="E15">
         <v>37541587.01752907</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>75157839.342062056</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>50040</v>
       </c>
@@ -2083,8 +2469,12 @@
       <c r="E16">
         <v>39780960.034711972</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>79585813.753807306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>50405</v>
       </c>
@@ -2100,8 +2490,12 @@
       <c r="E17">
         <v>41929905.526509926</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>83626452.129571423</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>50770</v>
       </c>
@@ -2117,8 +2511,12 @@
       <c r="E18">
         <v>43991417.091912232</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>87388236.848991394</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>51135</v>
       </c>
@@ -2134,8 +2532,12 @@
       <c r="E19">
         <v>45972334.145702273</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>91027659.880053729</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>51501</v>
       </c>
@@ -2151,8 +2553,12 @@
       <c r="E20">
         <v>47878551.280887984</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>94508547.571068212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>51866</v>
       </c>
@@ -2168,8 +2574,12 @@
       <c r="E21">
         <v>49688877.118642777</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>97643743.861070856</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>52231</v>
       </c>
@@ -2185,8 +2595,12 @@
       <c r="E22">
         <v>51370824.041904785</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>100391771.72030851</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>52596</v>
       </c>
@@ -2202,8 +2616,12 @@
       <c r="E23">
         <v>52920128.813968949</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>103014365.92962754</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>52962</v>
       </c>
@@ -2219,8 +2637,12 @@
       <c r="E24">
         <v>54364576.493288949</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>105531410.73979391</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>53327</v>
       </c>
@@ -2236,8 +2658,12 @@
       <c r="E25">
         <v>55690624.237227231</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>107623467.60497202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>53692</v>
       </c>
@@ -2253,8 +2679,12 @@
       <c r="E26">
         <v>56870661.085454665</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>109291096.91671294</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>54057</v>
       </c>
@@ -2270,8 +2700,12 @@
       <c r="E27">
         <v>57901126.505298585</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>110818111.44211438</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>54423</v>
       </c>
@@ -2287,8 +2721,12 @@
       <c r="E28">
         <v>58764914.32565318</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>111767759.8917255</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>54788</v>
       </c>
@@ -2304,8 +2742,12 @@
       <c r="E29">
         <v>59466380.726221606</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>112382112.50367118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>55153</v>
       </c>
@@ -2321,8 +2763,12 @@
       <c r="E30">
         <v>59996396.29226508</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>112511595.75122347</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>55518</v>
       </c>
@@ -2338,8 +2784,12 @@
       <c r="E31">
         <v>60316347.911723316</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>111999266.26208772</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>55884</v>
       </c>
@@ -2355,8 +2805,12 @@
       <c r="E32">
         <v>60408409.542703725</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>111300946.93618375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>56249</v>
       </c>
@@ -2372,8 +2826,12 @@
       <c r="E33">
         <v>60260587.801319174</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>109857631.47649178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>56614</v>
       </c>
@@ -2389,8 +2847,12 @@
       <c r="E34">
         <v>59872939.297520421</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>108083249.98784688</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>56979</v>
       </c>
@@ -2406,8 +2868,12 @@
       <c r="E35">
         <v>59238695.265142344</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>105945662.77932355</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>57345</v>
       </c>
@@ -2423,8 +2889,12 @@
       <c r="E36">
         <v>58351544.334336862</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>103467843.17359632</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>57710</v>
       </c>
@@ -2440,8 +2910,12 @@
       <c r="E37">
         <v>57220748.625263482</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>100808246.71792059</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>58075</v>
       </c>
@@ -2457,8 +2931,12 @@
       <c r="E38">
         <v>55828758.66093234</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>98015507.80796358</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>58440</v>
       </c>
@@ -2474,8 +2952,12 @@
       <c r="E39">
         <v>54196650.311278656</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>95225591.771610767</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>58806</v>
       </c>
@@ -2491,8 +2973,12 @@
       <c r="E40">
         <v>52397224.67017214</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>92280870.697095856</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>59171</v>
       </c>
@@ -2508,8 +2994,12 @@
       <c r="E41">
         <v>50476353.423770569</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>89029288.900285065</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>59536</v>
       </c>
@@ -2525,8 +3015,12 @@
       <c r="E42">
         <v>48451544.969263151</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>85465833.727939218</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>59901</v>
       </c>
@@ -2542,8 +3036,12 @@
       <c r="E43">
         <v>46340765.000131123</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>81885397.44734025</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>60267</v>
       </c>
@@ -2559,8 +3057,12 @@
       <c r="E44">
         <v>44172335.55584649</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>78418058.808885187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>60632</v>
       </c>
@@ -2576,8 +3078,12 @@
       <c r="E45">
         <v>41975845.765347295</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>74788358.425950393</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>60997</v>
       </c>
@@ -2593,8 +3099,12 @@
       <c r="E46">
         <v>39774557.724725142</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>70804081.119326591</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>61362</v>
       </c>
@@ -2610,8 +3120,12 @@
       <c r="E47">
         <v>37587076.486660495</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>66742539.109974474</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>61728</v>
       </c>
@@ -2627,8 +3141,12 @@
       <c r="E48">
         <v>35426194.380697556</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>62769008.254023343</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>62093</v>
       </c>
@@ -2644,8 +3162,12 @@
       <c r="E49">
         <v>33300674.862129819</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>58892570.929862916</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>62458</v>
       </c>
@@ -2661,8 +3183,12 @@
       <c r="E50">
         <v>31215161.836576086</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>55119280.671652094</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>62823</v>
       </c>
@@ -2678,8 +3204,12 @@
       <c r="E51">
         <v>29176454.786744218</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>51457141.955259517</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>63189</v>
       </c>
@@ -2695,8 +3225,12 @@
       <c r="E52">
         <v>27193199.561300345</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>47916216.67397891</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>63554</v>
       </c>
@@ -2712,8 +3246,12 @@
       <c r="E53">
         <v>25270062.080512874</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>44501512.584381439</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>63919</v>
       </c>
@@ -2729,8 +3267,12 @@
       <c r="E54">
         <v>23408630.367384732</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>41214363.22135599</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>64284</v>
       </c>
@@ -2746,8 +3288,12 @@
       <c r="E55">
         <v>21610641.685887225</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>38055959.646553934</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>64650</v>
       </c>
@@ -2763,8 +3309,12 @@
       <c r="E56">
         <v>19877734.39074285</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>35027136.265444927</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>65015</v>
       </c>
@@ -2780,8 +3330,12 @@
       <c r="E57">
         <v>18211438.843848299</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>32128417.38768293</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>65380</v>
       </c>
@@ -2797,8 +3351,12 @@
       <c r="E58">
         <v>16613456.139895046</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>29360334.656348888</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>65745</v>
       </c>
@@ -2814,8 +3372,12 @@
       <c r="E59">
         <v>15085669.45342824</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>26723457.578505002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>66111</v>
       </c>
@@ -2831,8 +3393,12 @@
       <c r="E60">
         <v>13630066.005969351</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>24218413.090876848</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>66476</v>
       </c>
@@ -2848,8 +3414,12 @@
       <c r="E61">
         <v>12248632.918981988</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>21845788.122647017</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>66841</v>
       </c>
@@ -2865,8 +3435,12 @@
       <c r="E62">
         <v>10943296.157121336</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>19606056.454499952</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>67206</v>
       </c>
@@ -2882,8 +3456,12 @@
       <c r="E63">
         <v>9715927.320641119</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>17499630.385934558</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>67572</v>
       </c>
@@ -2899,8 +3477,12 @@
       <c r="E64">
         <v>8568177.0788843464</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>15526752.41275485</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>67937</v>
       </c>
@@ -2916,8 +3498,12 @@
       <c r="E65">
         <v>7501367.6877569137</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>13687455.940023459</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>68302</v>
       </c>
@@ -2933,8 +3519,12 @@
       <c r="E66">
         <v>6516411.0252691954</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>11981561.807304464</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>68667</v>
       </c>
@@ -2950,8 +3540,12 @@
       <c r="E67">
         <v>5613737.3731370121</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <f t="shared" ref="F67:F81" si="1">SUM(C67:E67)</f>
+        <v>10408672.291602688</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>69033</v>
       </c>
@@ -2967,8 +3561,12 @@
       <c r="E68">
         <v>4793181.7741595935</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>8968042.7615011167</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>69398</v>
       </c>
@@ -2984,8 +3582,12 @@
       <c r="E69">
         <v>4053910.0508217267</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>7658539.0498977993</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69763</v>
       </c>
@@ -3001,8 +3603,12 @@
       <c r="E70">
         <v>3394354.6205073437</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>6478512.2317898646</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70128</v>
       </c>
@@ -3018,8 +3624,12 @@
       <c r="E71">
         <v>2812082.5552139655</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>5425367.9949210817</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70494</v>
       </c>
@@ -3035,8 +3645,12 @@
       <c r="E72">
         <v>2303717.901747026</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>4495160.2832379378</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>70859</v>
       </c>
@@ -3052,8 +3666,12 @@
       <c r="E73">
         <v>1865008.7193233322</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>3682514.1955013438</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>71224</v>
       </c>
@@ -3069,8 +3687,12 @@
       <c r="E74">
         <v>1490976.663464851</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>2980710.5997226508</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>71589</v>
       </c>
@@ -3086,8 +3708,12 @@
       <c r="E75">
         <v>1176068.601249408</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>2381734.5020340187</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>71955</v>
       </c>
@@ -3103,8 +3729,12 @@
       <c r="E76">
         <v>914425.98314517189</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>1876733.5989177078</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>72320</v>
       </c>
@@ -3120,8 +3750,12 @@
       <c r="E77">
         <v>700152.25580501626</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>1456704.8701808252</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>72685</v>
       </c>
@@ -3137,8 +3771,12 @@
       <c r="E78">
         <v>527400.94828807283</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>1112594.7415723156</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>73050</v>
       </c>
@@ -3154,8 +3792,12 @@
       <c r="E79">
         <v>390438.00132461288</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>835246.51611859258</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>73415</v>
       </c>
@@ -3171,8 +3813,12 @@
       <c r="E80">
         <v>283781.92345908063</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>615617.08377454244</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f>+EOMONTH(A80,12)</f>
         <v>73780</v>
@@ -3188,6 +3834,10 @@
       </c>
       <c r="E81">
         <v>202299.55102132255</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>444959.8221414939</v>
       </c>
     </row>
   </sheetData>
@@ -3199,7 +3849,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8773CC19-A081-4E73-B051-09B33C10AE79}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Began code for creating past cfs for liab mvs
</commit_message>
<xml_diff>
--- a/data/time_series/annual_cashflows_data.xlsx
+++ b/data/time_series/annual_cashflows_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\UPS_MV\data\time_series\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C54F7A-6559-4C96-8031-0C8D3F487BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800BE3C3-A949-49B1-85A7-35E395747081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3CCDB8E-F5F3-42E2-A382-F3745238F716}"/>
+    <workbookView xWindow="270" yWindow="375" windowWidth="16095" windowHeight="14565" xr2:uid="{F3CCDB8E-F5F3-42E2-A382-F3745238F716}"/>
   </bookViews>
   <sheets>
     <sheet name="PBO" sheetId="1" r:id="rId1"/>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027456B0-4AAC-4E49-B406-E9435788ACC8}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +441,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44926</v>
+        <v>44561</v>
       </c>
       <c r="B2">
         <v>0.5</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45291</v>
+        <v>44926</v>
       </c>
       <c r="B3">
         <v>1.5</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45657</v>
+        <v>45291</v>
       </c>
       <c r="B4">
         <v>2.5</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>46022</v>
+        <v>45657</v>
       </c>
       <c r="B5">
         <v>3.5</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>46387</v>
+        <v>46022</v>
       </c>
       <c r="B6">
         <v>4.5</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>46752</v>
+        <v>46387</v>
       </c>
       <c r="B7">
         <v>5.5</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>47118</v>
+        <v>46752</v>
       </c>
       <c r="B8">
         <v>6.5</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>47483</v>
+        <v>47118</v>
       </c>
       <c r="B9">
         <v>7.5</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>47848</v>
+        <v>47483</v>
       </c>
       <c r="B10">
         <v>8.5</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>48213</v>
+        <v>47848</v>
       </c>
       <c r="B11">
         <v>9.5</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>48579</v>
+        <v>48213</v>
       </c>
       <c r="B12">
         <v>10.5</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>48944</v>
+        <v>48579</v>
       </c>
       <c r="B13">
         <v>11.5</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>49309</v>
+        <v>48944</v>
       </c>
       <c r="B14">
         <v>12.5</v>
@@ -714,7 +714,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>49674</v>
+        <v>49309</v>
       </c>
       <c r="B15">
         <v>13.5</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>50040</v>
+        <v>49674</v>
       </c>
       <c r="B16">
         <v>14.5</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>50405</v>
+        <v>50040</v>
       </c>
       <c r="B17">
         <v>15.5</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>50770</v>
+        <v>50405</v>
       </c>
       <c r="B18">
         <v>16.5</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>51135</v>
+        <v>50770</v>
       </c>
       <c r="B19">
         <v>17.5</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>51501</v>
+        <v>51135</v>
       </c>
       <c r="B20">
         <v>18.5</v>
@@ -840,7 +840,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>51866</v>
+        <v>51501</v>
       </c>
       <c r="B21">
         <v>19.5</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>52231</v>
+        <v>51866</v>
       </c>
       <c r="B22">
         <v>20.5</v>
@@ -882,7 +882,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>52596</v>
+        <v>52231</v>
       </c>
       <c r="B23">
         <v>21.5</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>52962</v>
+        <v>52596</v>
       </c>
       <c r="B24">
         <v>22.5</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>53327</v>
+        <v>52962</v>
       </c>
       <c r="B25">
         <v>23.5</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>53692</v>
+        <v>53327</v>
       </c>
       <c r="B26">
         <v>24.5</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>54057</v>
+        <v>53692</v>
       </c>
       <c r="B27">
         <v>25.5</v>
@@ -987,7 +987,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>54423</v>
+        <v>54057</v>
       </c>
       <c r="B28">
         <v>26.5</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>54788</v>
+        <v>54423</v>
       </c>
       <c r="B29">
         <v>27.5</v>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>55153</v>
+        <v>54788</v>
       </c>
       <c r="B30">
         <v>28.5</v>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>55518</v>
+        <v>55153</v>
       </c>
       <c r="B31">
         <v>29.5</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>55884</v>
+        <v>55518</v>
       </c>
       <c r="B32">
         <v>30.5</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>56249</v>
+        <v>55884</v>
       </c>
       <c r="B33">
         <v>31.5</v>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>56614</v>
+        <v>56249</v>
       </c>
       <c r="B34">
         <v>32.5</v>
@@ -1134,7 +1134,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>56979</v>
+        <v>56614</v>
       </c>
       <c r="B35">
         <v>33.5</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>57345</v>
+        <v>56979</v>
       </c>
       <c r="B36">
         <v>34.5</v>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>57710</v>
+        <v>57345</v>
       </c>
       <c r="B37">
         <v>35.5</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>58075</v>
+        <v>57710</v>
       </c>
       <c r="B38">
         <v>36.5</v>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>58440</v>
+        <v>58075</v>
       </c>
       <c r="B39">
         <v>37.5</v>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>58806</v>
+        <v>58440</v>
       </c>
       <c r="B40">
         <v>38.5</v>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>59171</v>
+        <v>58806</v>
       </c>
       <c r="B41">
         <v>39.5</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>59536</v>
+        <v>59171</v>
       </c>
       <c r="B42">
         <v>40.5</v>
@@ -1302,7 +1302,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>59901</v>
+        <v>59536</v>
       </c>
       <c r="B43">
         <v>41.5</v>
@@ -1323,7 +1323,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>60267</v>
+        <v>59901</v>
       </c>
       <c r="B44">
         <v>42.5</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>60632</v>
+        <v>60267</v>
       </c>
       <c r="B45">
         <v>43.5</v>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>60997</v>
+        <v>60632</v>
       </c>
       <c r="B46">
         <v>44.5</v>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>61362</v>
+        <v>60997</v>
       </c>
       <c r="B47">
         <v>45.5</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>61728</v>
+        <v>61362</v>
       </c>
       <c r="B48">
         <v>46.5</v>
@@ -1428,7 +1428,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>62093</v>
+        <v>61728</v>
       </c>
       <c r="B49">
         <v>47.5</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>62458</v>
+        <v>62093</v>
       </c>
       <c r="B50">
         <v>48.5</v>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>62823</v>
+        <v>62458</v>
       </c>
       <c r="B51">
         <v>49.5</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>63189</v>
+        <v>62823</v>
       </c>
       <c r="B52">
         <v>50.5</v>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>63554</v>
+        <v>63189</v>
       </c>
       <c r="B53">
         <v>51.5</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>63919</v>
+        <v>63554</v>
       </c>
       <c r="B54">
         <v>52.5</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>64284</v>
+        <v>63919</v>
       </c>
       <c r="B55">
         <v>53.5</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>64650</v>
+        <v>64284</v>
       </c>
       <c r="B56">
         <v>54.5</v>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>65015</v>
+        <v>64650</v>
       </c>
       <c r="B57">
         <v>55.5</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>65380</v>
+        <v>65015</v>
       </c>
       <c r="B58">
         <v>56.5</v>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>65745</v>
+        <v>65380</v>
       </c>
       <c r="B59">
         <v>57.5</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>66111</v>
+        <v>65745</v>
       </c>
       <c r="B60">
         <v>58.5</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>66476</v>
+        <v>66111</v>
       </c>
       <c r="B61">
         <v>59.5</v>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>66841</v>
+        <v>66476</v>
       </c>
       <c r="B62">
         <v>60.5</v>
@@ -1722,7 +1722,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>67206</v>
+        <v>66841</v>
       </c>
       <c r="B63">
         <v>61.5</v>
@@ -1743,7 +1743,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>67572</v>
+        <v>67206</v>
       </c>
       <c r="B64">
         <v>62.5</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>67937</v>
+        <v>67572</v>
       </c>
       <c r="B65">
         <v>63.5</v>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>68302</v>
+        <v>67937</v>
       </c>
       <c r="B66">
         <v>64.5</v>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>68667</v>
+        <v>68302</v>
       </c>
       <c r="B67">
         <v>65.5</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>69033</v>
+        <v>68667</v>
       </c>
       <c r="B68">
         <v>66.5</v>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>69398</v>
+        <v>69033</v>
       </c>
       <c r="B69">
         <v>67.5</v>
@@ -1869,7 +1869,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>69763</v>
+        <v>69398</v>
       </c>
       <c r="B70">
         <v>68.5</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>70128</v>
+        <v>69763</v>
       </c>
       <c r="B71">
         <v>69.5</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>70494</v>
+        <v>70128</v>
       </c>
       <c r="B72">
         <v>70.5</v>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>70859</v>
+        <v>70494</v>
       </c>
       <c r="B73">
         <v>71.5</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>71224</v>
+        <v>70859</v>
       </c>
       <c r="B74">
         <v>72.5</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>71589</v>
+        <v>71224</v>
       </c>
       <c r="B75">
         <v>73.5</v>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>71955</v>
+        <v>71589</v>
       </c>
       <c r="B76">
         <v>74.5</v>
@@ -2016,7 +2016,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>72320</v>
+        <v>71955</v>
       </c>
       <c r="B77">
         <v>75.5</v>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>72685</v>
+        <v>72320</v>
       </c>
       <c r="B78">
         <v>76.5</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>73050</v>
+        <v>72685</v>
       </c>
       <c r="B79">
         <v>77.5</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>73415</v>
+        <v>73050</v>
       </c>
       <c r="B80">
         <v>78.5</v>
@@ -2100,8 +2100,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <f>+EOMONTH(A80,12)</f>
-        <v>73780</v>
+        <v>73415</v>
       </c>
       <c r="B81">
         <v>79.5</v>
@@ -2129,8 +2128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B07887-8F52-4ACD-9003-CB270BD2655C}">
   <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,7 +2160,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44926</v>
+        <v>44561</v>
       </c>
       <c r="B2">
         <v>0.5</v>
@@ -2182,7 +2181,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45291</v>
+        <v>44926</v>
       </c>
       <c r="B3">
         <v>1.5</v>
@@ -2203,7 +2202,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45657</v>
+        <v>45291</v>
       </c>
       <c r="B4">
         <v>2.5</v>
@@ -2224,7 +2223,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>46022</v>
+        <v>45657</v>
       </c>
       <c r="B5">
         <v>3.5</v>
@@ -2245,7 +2244,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>46387</v>
+        <v>46022</v>
       </c>
       <c r="B6">
         <v>4.5</v>
@@ -2266,7 +2265,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>46752</v>
+        <v>46387</v>
       </c>
       <c r="B7">
         <v>5.5</v>
@@ -2287,7 +2286,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>47118</v>
+        <v>46752</v>
       </c>
       <c r="B8">
         <v>6.5</v>
@@ -2308,7 +2307,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>47483</v>
+        <v>47118</v>
       </c>
       <c r="B9">
         <v>7.5</v>
@@ -2329,7 +2328,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>47848</v>
+        <v>47483</v>
       </c>
       <c r="B10">
         <v>8.5</v>
@@ -2350,7 +2349,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>48213</v>
+        <v>47848</v>
       </c>
       <c r="B11">
         <v>9.5</v>
@@ -2371,7 +2370,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>48579</v>
+        <v>48213</v>
       </c>
       <c r="B12">
         <v>10.5</v>
@@ -2392,7 +2391,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>48944</v>
+        <v>48579</v>
       </c>
       <c r="B13">
         <v>11.5</v>
@@ -2413,7 +2412,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>49309</v>
+        <v>48944</v>
       </c>
       <c r="B14">
         <v>12.5</v>
@@ -2434,7 +2433,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>49674</v>
+        <v>49309</v>
       </c>
       <c r="B15">
         <v>13.5</v>
@@ -2455,7 +2454,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>50040</v>
+        <v>49674</v>
       </c>
       <c r="B16">
         <v>14.5</v>
@@ -2476,7 +2475,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>50405</v>
+        <v>50040</v>
       </c>
       <c r="B17">
         <v>15.5</v>
@@ -2497,7 +2496,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>50770</v>
+        <v>50405</v>
       </c>
       <c r="B18">
         <v>16.5</v>
@@ -2518,7 +2517,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>51135</v>
+        <v>50770</v>
       </c>
       <c r="B19">
         <v>17.5</v>
@@ -2539,7 +2538,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>51501</v>
+        <v>51135</v>
       </c>
       <c r="B20">
         <v>18.5</v>
@@ -2560,7 +2559,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>51866</v>
+        <v>51501</v>
       </c>
       <c r="B21">
         <v>19.5</v>
@@ -2581,7 +2580,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>52231</v>
+        <v>51866</v>
       </c>
       <c r="B22">
         <v>20.5</v>
@@ -2602,7 +2601,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>52596</v>
+        <v>52231</v>
       </c>
       <c r="B23">
         <v>21.5</v>
@@ -2623,7 +2622,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>52962</v>
+        <v>52596</v>
       </c>
       <c r="B24">
         <v>22.5</v>
@@ -2644,7 +2643,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>53327</v>
+        <v>52962</v>
       </c>
       <c r="B25">
         <v>23.5</v>
@@ -2665,7 +2664,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>53692</v>
+        <v>53327</v>
       </c>
       <c r="B26">
         <v>24.5</v>
@@ -2686,7 +2685,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>54057</v>
+        <v>53692</v>
       </c>
       <c r="B27">
         <v>25.5</v>
@@ -2707,7 +2706,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>54423</v>
+        <v>54057</v>
       </c>
       <c r="B28">
         <v>26.5</v>
@@ -2728,7 +2727,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>54788</v>
+        <v>54423</v>
       </c>
       <c r="B29">
         <v>27.5</v>
@@ -2749,7 +2748,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>55153</v>
+        <v>54788</v>
       </c>
       <c r="B30">
         <v>28.5</v>
@@ -2770,7 +2769,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>55518</v>
+        <v>55153</v>
       </c>
       <c r="B31">
         <v>29.5</v>
@@ -2791,7 +2790,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>55884</v>
+        <v>55518</v>
       </c>
       <c r="B32">
         <v>30.5</v>
@@ -2812,7 +2811,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>56249</v>
+        <v>55884</v>
       </c>
       <c r="B33">
         <v>31.5</v>
@@ -2833,7 +2832,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>56614</v>
+        <v>56249</v>
       </c>
       <c r="B34">
         <v>32.5</v>
@@ -2854,7 +2853,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>56979</v>
+        <v>56614</v>
       </c>
       <c r="B35">
         <v>33.5</v>
@@ -2875,7 +2874,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>57345</v>
+        <v>56979</v>
       </c>
       <c r="B36">
         <v>34.5</v>
@@ -2896,7 +2895,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>57710</v>
+        <v>57345</v>
       </c>
       <c r="B37">
         <v>35.5</v>
@@ -2917,7 +2916,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>58075</v>
+        <v>57710</v>
       </c>
       <c r="B38">
         <v>36.5</v>
@@ -2938,7 +2937,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>58440</v>
+        <v>58075</v>
       </c>
       <c r="B39">
         <v>37.5</v>
@@ -2959,7 +2958,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>58806</v>
+        <v>58440</v>
       </c>
       <c r="B40">
         <v>38.5</v>
@@ -2980,7 +2979,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>59171</v>
+        <v>58806</v>
       </c>
       <c r="B41">
         <v>39.5</v>
@@ -3001,7 +3000,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>59536</v>
+        <v>59171</v>
       </c>
       <c r="B42">
         <v>40.5</v>
@@ -3022,7 +3021,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>59901</v>
+        <v>59536</v>
       </c>
       <c r="B43">
         <v>41.5</v>
@@ -3043,7 +3042,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>60267</v>
+        <v>59901</v>
       </c>
       <c r="B44">
         <v>42.5</v>
@@ -3064,7 +3063,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>60632</v>
+        <v>60267</v>
       </c>
       <c r="B45">
         <v>43.5</v>
@@ -3085,7 +3084,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>60997</v>
+        <v>60632</v>
       </c>
       <c r="B46">
         <v>44.5</v>
@@ -3106,7 +3105,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>61362</v>
+        <v>60997</v>
       </c>
       <c r="B47">
         <v>45.5</v>
@@ -3127,7 +3126,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>61728</v>
+        <v>61362</v>
       </c>
       <c r="B48">
         <v>46.5</v>
@@ -3148,7 +3147,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>62093</v>
+        <v>61728</v>
       </c>
       <c r="B49">
         <v>47.5</v>
@@ -3169,7 +3168,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>62458</v>
+        <v>62093</v>
       </c>
       <c r="B50">
         <v>48.5</v>
@@ -3190,7 +3189,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>62823</v>
+        <v>62458</v>
       </c>
       <c r="B51">
         <v>49.5</v>
@@ -3211,7 +3210,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>63189</v>
+        <v>62823</v>
       </c>
       <c r="B52">
         <v>50.5</v>
@@ -3232,7 +3231,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>63554</v>
+        <v>63189</v>
       </c>
       <c r="B53">
         <v>51.5</v>
@@ -3253,7 +3252,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>63919</v>
+        <v>63554</v>
       </c>
       <c r="B54">
         <v>52.5</v>
@@ -3274,7 +3273,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>64284</v>
+        <v>63919</v>
       </c>
       <c r="B55">
         <v>53.5</v>
@@ -3295,7 +3294,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>64650</v>
+        <v>64284</v>
       </c>
       <c r="B56">
         <v>54.5</v>
@@ -3316,7 +3315,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>65015</v>
+        <v>64650</v>
       </c>
       <c r="B57">
         <v>55.5</v>
@@ -3337,7 +3336,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>65380</v>
+        <v>65015</v>
       </c>
       <c r="B58">
         <v>56.5</v>
@@ -3358,7 +3357,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>65745</v>
+        <v>65380</v>
       </c>
       <c r="B59">
         <v>57.5</v>
@@ -3379,7 +3378,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>66111</v>
+        <v>65745</v>
       </c>
       <c r="B60">
         <v>58.5</v>
@@ -3400,7 +3399,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>66476</v>
+        <v>66111</v>
       </c>
       <c r="B61">
         <v>59.5</v>
@@ -3421,7 +3420,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>66841</v>
+        <v>66476</v>
       </c>
       <c r="B62">
         <v>60.5</v>
@@ -3442,7 +3441,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>67206</v>
+        <v>66841</v>
       </c>
       <c r="B63">
         <v>61.5</v>
@@ -3463,7 +3462,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>67572</v>
+        <v>67206</v>
       </c>
       <c r="B64">
         <v>62.5</v>
@@ -3484,7 +3483,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>67937</v>
+        <v>67572</v>
       </c>
       <c r="B65">
         <v>63.5</v>
@@ -3505,7 +3504,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>68302</v>
+        <v>67937</v>
       </c>
       <c r="B66">
         <v>64.5</v>
@@ -3526,7 +3525,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>68667</v>
+        <v>68302</v>
       </c>
       <c r="B67">
         <v>65.5</v>
@@ -3547,7 +3546,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>69033</v>
+        <v>68667</v>
       </c>
       <c r="B68">
         <v>66.5</v>
@@ -3568,7 +3567,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>69398</v>
+        <v>69033</v>
       </c>
       <c r="B69">
         <v>67.5</v>
@@ -3589,7 +3588,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>69763</v>
+        <v>69398</v>
       </c>
       <c r="B70">
         <v>68.5</v>
@@ -3610,7 +3609,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>70128</v>
+        <v>69763</v>
       </c>
       <c r="B71">
         <v>69.5</v>
@@ -3631,7 +3630,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>70494</v>
+        <v>70128</v>
       </c>
       <c r="B72">
         <v>70.5</v>
@@ -3652,7 +3651,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>70859</v>
+        <v>70494</v>
       </c>
       <c r="B73">
         <v>71.5</v>
@@ -3673,7 +3672,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>71224</v>
+        <v>70859</v>
       </c>
       <c r="B74">
         <v>72.5</v>
@@ -3694,7 +3693,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>71589</v>
+        <v>71224</v>
       </c>
       <c r="B75">
         <v>73.5</v>
@@ -3715,7 +3714,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>71955</v>
+        <v>71589</v>
       </c>
       <c r="B76">
         <v>74.5</v>
@@ -3736,7 +3735,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>72320</v>
+        <v>71955</v>
       </c>
       <c r="B77">
         <v>75.5</v>
@@ -3757,7 +3756,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>72685</v>
+        <v>72320</v>
       </c>
       <c r="B78">
         <v>76.5</v>
@@ -3778,7 +3777,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>73050</v>
+        <v>72685</v>
       </c>
       <c r="B79">
         <v>77.5</v>
@@ -3799,7 +3798,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>73415</v>
+        <v>73050</v>
       </c>
       <c r="B80">
         <v>78.5</v>
@@ -3820,8 +3819,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <f>+EOMONTH(A80,12)</f>
-        <v>73780</v>
+        <v>73415</v>
       </c>
       <c r="B81">
         <v>79.5</v>

</xml_diff>